<commit_message>
Publish senate primary overview
</commit_message>
<xml_diff>
--- a/_data/2020/MA_State_Senate_Race_2022.xlsx
+++ b/_data/2020/MA_State_Senate_Race_2022.xlsx
@@ -1,14 +1,14 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10611"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10814"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/bbenson/Documents/Research/ma_2022/post/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/bbenson/Documents/Research/massnumbers_blog/blog/_data/2020/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{401748AE-60EF-9047-9A25-AF75A376DF5C}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{8F894862-7D2E-994D-AF6C-2666F1AEB940}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="500" windowWidth="32560" windowHeight="20500" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -125,9 +125,6 @@
     <t>D+4</t>
   </si>
   <si>
-    <t>(Eric Lesser—Longmeadow)</t>
-  </si>
-  <si>
     <t>D,R</t>
   </si>
   <si>
@@ -182,9 +179,6 @@
     <t>D+17</t>
   </si>
   <si>
-    <t>(Harriette L. Chandler—Worcester)</t>
-  </si>
-  <si>
     <t>Worcester and Middlesex</t>
   </si>
   <si>
@@ -269,9 +263,6 @@
     <t>D+15</t>
   </si>
   <si>
-    <t>(Diana DiZoglio—Methuen)</t>
-  </si>
-  <si>
     <t>Second Essex and Middlesex</t>
   </si>
   <si>
@@ -347,9 +338,6 @@
     <t>D+42</t>
   </si>
   <si>
-    <t>(Sonia Chang-Diaz—Boston)</t>
-  </si>
-  <si>
     <t>First Suffolk</t>
   </si>
   <si>
@@ -368,9 +356,6 @@
     <t>D+9</t>
   </si>
   <si>
-    <t>Patrick Michael O'Connor—Weymouth</t>
-  </si>
-  <si>
     <t>R</t>
   </si>
   <si>
@@ -1946,7 +1931,22 @@
     <t>1992-05-27</t>
   </si>
   <si>
-    <t>(Adam Hinds—Pittsfield)</t>
+    <t>Patrick O'Connor—Weymouth</t>
+  </si>
+  <si>
+    <t>(Adam Hinds—Pittsfield)*</t>
+  </si>
+  <si>
+    <t>(Eric Lesser—Longmeadow)*</t>
+  </si>
+  <si>
+    <t>(Harriette L. Chandler—Worcester)*</t>
+  </si>
+  <si>
+    <t>(Diana DiZoglio—Methuen)*</t>
+  </si>
+  <si>
+    <t>(Sonia Chang-Diaz—Boston)*</t>
   </si>
 </sst>
 </file>
@@ -2397,7 +2397,7 @@
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
       <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="H3" sqref="H3"/>
+      <selection pane="bottomLeft" activeCell="A2" sqref="A2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="12.6640625" defaultRowHeight="15.75" customHeight="1" x14ac:dyDescent="0.15"/>
@@ -2496,7 +2496,7 @@
         <v>17</v>
       </c>
       <c r="H2" s="12" t="s">
-        <v>637</v>
+        <v>633</v>
       </c>
       <c r="I2" s="15">
         <v>0.95799999999999996</v>
@@ -2624,13 +2624,13 @@
         <v>17</v>
       </c>
       <c r="H5" s="12" t="s">
-        <v>30</v>
+        <v>634</v>
       </c>
       <c r="I5" s="15">
         <v>0.57599999999999996</v>
       </c>
       <c r="J5" s="16" t="s">
-        <v>31</v>
+        <v>30</v>
       </c>
       <c r="K5" s="11">
         <v>4</v>
@@ -2650,10 +2650,10 @@
         <v>5</v>
       </c>
       <c r="B6" s="11" t="s">
-        <v>32</v>
+        <v>31</v>
       </c>
       <c r="C6" s="12" t="s">
-        <v>32</v>
+        <v>31</v>
       </c>
       <c r="D6" s="13">
         <v>0.80380402970443598</v>
@@ -2662,13 +2662,13 @@
         <v>22.563926054475399</v>
       </c>
       <c r="F6" s="10" t="s">
-        <v>33</v>
+        <v>32</v>
       </c>
       <c r="G6" s="11" t="s">
         <v>22</v>
       </c>
       <c r="H6" s="12" t="s">
-        <v>34</v>
+        <v>33</v>
       </c>
       <c r="I6" s="15">
         <v>1</v>
@@ -2692,10 +2692,10 @@
         <v>6</v>
       </c>
       <c r="B7" s="11" t="s">
+        <v>34</v>
+      </c>
+      <c r="C7" s="12" t="s">
         <v>35</v>
-      </c>
-      <c r="C7" s="12" t="s">
-        <v>36</v>
       </c>
       <c r="D7" s="13">
         <v>0.85282172108156595</v>
@@ -2704,13 +2704,13 @@
         <v>-8.0370288947828605E-2</v>
       </c>
       <c r="F7" s="10" t="s">
-        <v>37</v>
+        <v>36</v>
       </c>
       <c r="G7" s="11" t="s">
         <v>22</v>
       </c>
       <c r="H7" s="12" t="s">
-        <v>38</v>
+        <v>37</v>
       </c>
       <c r="I7" s="15">
         <v>0.84399999999999997</v>
@@ -2734,10 +2734,10 @@
         <v>7</v>
       </c>
       <c r="B8" s="11" t="s">
+        <v>38</v>
+      </c>
+      <c r="C8" s="12" t="s">
         <v>39</v>
-      </c>
-      <c r="C8" s="12" t="s">
-        <v>40</v>
       </c>
       <c r="D8" s="13">
         <v>0.86451381116223802</v>
@@ -2746,13 +2746,13 @@
         <v>-2.4861715862562801</v>
       </c>
       <c r="F8" s="10" t="s">
+        <v>40</v>
+      </c>
+      <c r="G8" s="11" t="s">
         <v>41</v>
       </c>
-      <c r="G8" s="11" t="s">
+      <c r="H8" s="12" t="s">
         <v>42</v>
-      </c>
-      <c r="H8" s="12" t="s">
-        <v>43</v>
       </c>
       <c r="I8" s="15">
         <v>0</v>
@@ -2776,10 +2776,10 @@
         <v>8</v>
       </c>
       <c r="B9" s="11" t="s">
-        <v>44</v>
+        <v>43</v>
       </c>
       <c r="C9" s="12" t="s">
-        <v>44</v>
+        <v>43</v>
       </c>
       <c r="D9" s="13">
         <v>0.67837019754950101</v>
@@ -2788,13 +2788,13 @@
         <v>10.944685306667999</v>
       </c>
       <c r="F9" s="10" t="s">
-        <v>45</v>
+        <v>44</v>
       </c>
       <c r="G9" s="11" t="s">
         <v>22</v>
       </c>
       <c r="H9" s="12" t="s">
-        <v>46</v>
+        <v>45</v>
       </c>
       <c r="I9" s="15">
         <v>1</v>
@@ -2818,10 +2818,10 @@
         <v>9</v>
       </c>
       <c r="B10" s="11" t="s">
-        <v>47</v>
+        <v>46</v>
       </c>
       <c r="C10" s="12" t="s">
-        <v>47</v>
+        <v>46</v>
       </c>
       <c r="D10" s="13">
         <v>0.59623136285307499</v>
@@ -2830,13 +2830,13 @@
         <v>17.235286066614101</v>
       </c>
       <c r="F10" s="10" t="s">
-        <v>48</v>
+        <v>47</v>
       </c>
       <c r="G10" s="11" t="s">
         <v>17</v>
       </c>
       <c r="H10" s="12" t="s">
-        <v>49</v>
+        <v>635</v>
       </c>
       <c r="I10" s="15">
         <v>0.95599999999999996</v>
@@ -2862,10 +2862,10 @@
         <v>10</v>
       </c>
       <c r="B11" s="11" t="s">
-        <v>50</v>
+        <v>48</v>
       </c>
       <c r="C11" s="12" t="s">
-        <v>50</v>
+        <v>48</v>
       </c>
       <c r="D11" s="13">
         <v>0.72413026484699405</v>
@@ -2874,13 +2874,13 @@
         <v>7.50568958047882</v>
       </c>
       <c r="F11" s="10" t="s">
-        <v>51</v>
+        <v>49</v>
       </c>
       <c r="G11" s="11" t="s">
         <v>22</v>
       </c>
       <c r="H11" s="12" t="s">
-        <v>52</v>
+        <v>50</v>
       </c>
       <c r="I11" s="15">
         <v>0.94299999999999995</v>
@@ -2904,10 +2904,10 @@
         <v>11</v>
       </c>
       <c r="B12" s="11" t="s">
-        <v>53</v>
+        <v>51</v>
       </c>
       <c r="C12" s="12" t="s">
-        <v>53</v>
+        <v>51</v>
       </c>
       <c r="D12" s="13">
         <v>0.58027228172082002</v>
@@ -2916,13 +2916,13 @@
         <v>7.84478328395695</v>
       </c>
       <c r="F12" s="10" t="s">
-        <v>51</v>
+        <v>49</v>
       </c>
       <c r="G12" s="11" t="s">
         <v>22</v>
       </c>
       <c r="H12" s="12" t="s">
-        <v>54</v>
+        <v>52</v>
       </c>
       <c r="I12" s="15">
         <v>1</v>
@@ -2946,10 +2946,10 @@
         <v>12</v>
       </c>
       <c r="B13" s="11" t="s">
-        <v>55</v>
+        <v>53</v>
       </c>
       <c r="C13" s="12" t="s">
-        <v>55</v>
+        <v>53</v>
       </c>
       <c r="D13" s="13">
         <v>0.74784155307367095</v>
@@ -2958,13 +2958,13 @@
         <v>19.759362509721299</v>
       </c>
       <c r="F13" s="10" t="s">
-        <v>56</v>
+        <v>54</v>
       </c>
       <c r="G13" s="11" t="s">
         <v>22</v>
       </c>
       <c r="H13" s="12" t="s">
-        <v>57</v>
+        <v>55</v>
       </c>
       <c r="I13" s="15">
         <v>0.99399999999999999</v>
@@ -2988,10 +2988,10 @@
         <v>13</v>
       </c>
       <c r="B14" s="11" t="s">
-        <v>58</v>
+        <v>56</v>
       </c>
       <c r="C14" s="12" t="s">
-        <v>59</v>
+        <v>57</v>
       </c>
       <c r="D14" s="13">
         <v>0.69770721031681904</v>
@@ -3000,13 +3000,13 @@
         <v>20.067051243839799</v>
       </c>
       <c r="F14" s="10" t="s">
-        <v>56</v>
+        <v>54</v>
       </c>
       <c r="G14" s="11" t="s">
         <v>22</v>
       </c>
       <c r="H14" s="12" t="s">
-        <v>60</v>
+        <v>58</v>
       </c>
       <c r="I14" s="15">
         <v>1</v>
@@ -3030,10 +3030,10 @@
         <v>14</v>
       </c>
       <c r="B15" s="11" t="s">
-        <v>61</v>
+        <v>59</v>
       </c>
       <c r="C15" s="12" t="s">
-        <v>62</v>
+        <v>60</v>
       </c>
       <c r="D15" s="13">
         <v>0.83668814132462599</v>
@@ -3042,13 +3042,13 @@
         <v>11.559096920657099</v>
       </c>
       <c r="F15" s="10" t="s">
-        <v>63</v>
+        <v>61</v>
       </c>
       <c r="G15" s="11" t="s">
         <v>22</v>
       </c>
       <c r="H15" s="12" t="s">
-        <v>64</v>
+        <v>62</v>
       </c>
       <c r="I15" s="15">
         <v>0.97799999999999998</v>
@@ -3072,10 +3072,10 @@
         <v>15</v>
       </c>
       <c r="B16" s="11" t="s">
-        <v>65</v>
+        <v>63</v>
       </c>
       <c r="C16" s="12" t="s">
-        <v>65</v>
+        <v>63</v>
       </c>
       <c r="D16" s="13">
         <v>0.71918507924462205</v>
@@ -3084,13 +3084,13 @@
         <v>20.439302890255199</v>
       </c>
       <c r="F16" s="10" t="s">
-        <v>56</v>
+        <v>54</v>
       </c>
       <c r="G16" s="11" t="s">
         <v>22</v>
       </c>
       <c r="H16" s="12" t="s">
-        <v>66</v>
+        <v>64</v>
       </c>
       <c r="I16" s="15">
         <v>1</v>
@@ -3114,10 +3114,10 @@
         <v>16</v>
       </c>
       <c r="B17" s="11" t="s">
-        <v>67</v>
+        <v>65</v>
       </c>
       <c r="C17" s="11" t="s">
-        <v>67</v>
+        <v>65</v>
       </c>
       <c r="D17" s="13">
         <v>0.75370953237409999</v>
@@ -3126,13 +3126,13 @@
         <v>15.7644112052139</v>
       </c>
       <c r="F17" s="10" t="s">
-        <v>68</v>
+        <v>66</v>
       </c>
       <c r="G17" s="11" t="s">
         <v>22</v>
       </c>
       <c r="H17" s="12" t="s">
-        <v>69</v>
+        <v>67</v>
       </c>
       <c r="I17" s="15">
         <v>1</v>
@@ -3156,10 +3156,10 @@
         <v>17</v>
       </c>
       <c r="B18" s="11" t="s">
-        <v>70</v>
+        <v>68</v>
       </c>
       <c r="C18" s="12" t="s">
-        <v>71</v>
+        <v>69</v>
       </c>
       <c r="D18" s="13">
         <v>0.71132627472833598</v>
@@ -3168,13 +3168,13 @@
         <v>32.146847770266803</v>
       </c>
       <c r="F18" s="10" t="s">
-        <v>72</v>
+        <v>70</v>
       </c>
       <c r="G18" s="11" t="s">
         <v>22</v>
       </c>
       <c r="H18" s="12" t="s">
-        <v>73</v>
+        <v>71</v>
       </c>
       <c r="I18" s="15">
         <v>0.999</v>
@@ -3198,10 +3198,10 @@
         <v>18</v>
       </c>
       <c r="B19" s="11" t="s">
-        <v>74</v>
+        <v>72</v>
       </c>
       <c r="C19" s="11" t="s">
-        <v>74</v>
+        <v>72</v>
       </c>
       <c r="D19" s="13">
         <v>0.70610800667511397</v>
@@ -3216,7 +3216,7 @@
         <v>22</v>
       </c>
       <c r="H19" s="12" t="s">
-        <v>75</v>
+        <v>73</v>
       </c>
       <c r="I19" s="15">
         <v>1</v>
@@ -3240,10 +3240,10 @@
         <v>19</v>
       </c>
       <c r="B20" s="11" t="s">
-        <v>76</v>
+        <v>74</v>
       </c>
       <c r="C20" s="12" t="s">
-        <v>76</v>
+        <v>74</v>
       </c>
       <c r="D20" s="13">
         <v>0.360955910825911</v>
@@ -3252,13 +3252,13 @@
         <v>15.2551501274617</v>
       </c>
       <c r="F20" s="10" t="s">
-        <v>77</v>
+        <v>75</v>
       </c>
       <c r="G20" s="11" t="s">
         <v>17</v>
       </c>
       <c r="H20" s="12" t="s">
-        <v>78</v>
+        <v>636</v>
       </c>
       <c r="I20" s="15">
         <v>1</v>
@@ -3284,10 +3284,10 @@
         <v>20</v>
       </c>
       <c r="B21" s="11" t="s">
-        <v>79</v>
+        <v>76</v>
       </c>
       <c r="C21" s="11" t="s">
-        <v>79</v>
+        <v>76</v>
       </c>
       <c r="D21" s="13">
         <v>0.83802388587858001</v>
@@ -3302,7 +3302,7 @@
         <v>22</v>
       </c>
       <c r="H21" s="12" t="s">
-        <v>80</v>
+        <v>77</v>
       </c>
       <c r="I21" s="15">
         <v>0.92300000000000004</v>
@@ -3326,10 +3326,10 @@
         <v>21</v>
       </c>
       <c r="B22" s="11" t="s">
-        <v>81</v>
+        <v>78</v>
       </c>
       <c r="C22" s="11" t="s">
-        <v>81</v>
+        <v>78</v>
       </c>
       <c r="D22" s="13">
         <v>0.90920350937553696</v>
@@ -3338,13 +3338,13 @@
         <v>9.9724578971641797</v>
       </c>
       <c r="F22" s="10" t="s">
-        <v>82</v>
+        <v>79</v>
       </c>
       <c r="G22" s="11" t="s">
-        <v>42</v>
+        <v>41</v>
       </c>
       <c r="H22" s="12" t="s">
-        <v>83</v>
+        <v>80</v>
       </c>
       <c r="I22" s="15">
         <v>0</v>
@@ -3368,10 +3368,10 @@
         <v>22</v>
       </c>
       <c r="B23" s="11" t="s">
-        <v>84</v>
+        <v>81</v>
       </c>
       <c r="C23" s="11" t="s">
-        <v>84</v>
+        <v>81</v>
       </c>
       <c r="D23" s="13">
         <v>0.81527884862503197</v>
@@ -3380,13 +3380,13 @@
         <v>12.212307616672</v>
       </c>
       <c r="F23" s="10" t="s">
-        <v>63</v>
+        <v>61</v>
       </c>
       <c r="G23" s="11" t="s">
         <v>22</v>
       </c>
       <c r="H23" s="12" t="s">
-        <v>85</v>
+        <v>82</v>
       </c>
       <c r="I23" s="15">
         <v>0.97199999999999998</v>
@@ -3412,10 +3412,10 @@
         <v>23</v>
       </c>
       <c r="B24" s="11" t="s">
-        <v>86</v>
+        <v>83</v>
       </c>
       <c r="C24" s="11" t="s">
-        <v>86</v>
+        <v>83</v>
       </c>
       <c r="D24" s="13">
         <v>0.68586643150289905</v>
@@ -3424,13 +3424,13 @@
         <v>16.087056323342601</v>
       </c>
       <c r="F24" s="10" t="s">
-        <v>68</v>
+        <v>66</v>
       </c>
       <c r="G24" s="11" t="s">
         <v>22</v>
       </c>
       <c r="H24" s="12" t="s">
-        <v>87</v>
+        <v>84</v>
       </c>
       <c r="I24" s="15">
         <v>0.98699999999999999</v>
@@ -3454,10 +3454,10 @@
         <v>24</v>
       </c>
       <c r="B25" s="11" t="s">
-        <v>88</v>
+        <v>85</v>
       </c>
       <c r="C25" s="11" t="s">
-        <v>88</v>
+        <v>85</v>
       </c>
       <c r="D25" s="13">
         <v>0.60495618527369899</v>
@@ -3466,13 +3466,13 @@
         <v>12.558164731909301</v>
       </c>
       <c r="F25" s="10" t="s">
-        <v>89</v>
+        <v>86</v>
       </c>
       <c r="G25" s="11" t="s">
         <v>22</v>
       </c>
       <c r="H25" s="12" t="s">
-        <v>90</v>
+        <v>87</v>
       </c>
       <c r="I25" s="15">
         <v>0.98099999999999998</v>
@@ -3496,10 +3496,10 @@
         <v>25</v>
       </c>
       <c r="B26" s="11" t="s">
-        <v>91</v>
+        <v>88</v>
       </c>
       <c r="C26" s="12" t="s">
-        <v>92</v>
+        <v>89</v>
       </c>
       <c r="D26" s="13">
         <v>0.58576026879031495</v>
@@ -3508,13 +3508,13 @@
         <v>21.115611005947301</v>
       </c>
       <c r="F26" s="10" t="s">
-        <v>93</v>
+        <v>90</v>
       </c>
       <c r="G26" s="11" t="s">
         <v>22</v>
       </c>
       <c r="H26" s="12" t="s">
-        <v>94</v>
+        <v>91</v>
       </c>
       <c r="I26" s="15">
         <v>1</v>
@@ -3538,10 +3538,10 @@
         <v>26</v>
       </c>
       <c r="B27" s="11" t="s">
-        <v>95</v>
+        <v>92</v>
       </c>
       <c r="C27" s="11" t="s">
-        <v>95</v>
+        <v>92</v>
       </c>
       <c r="D27" s="13">
         <v>0.45667208047362001</v>
@@ -3550,13 +3550,13 @@
         <v>32.340137539069502</v>
       </c>
       <c r="F27" s="10" t="s">
-        <v>72</v>
+        <v>70</v>
       </c>
       <c r="G27" s="11" t="s">
         <v>22</v>
       </c>
       <c r="H27" s="12" t="s">
-        <v>96</v>
+        <v>93</v>
       </c>
       <c r="I27" s="15">
         <v>1</v>
@@ -3580,10 +3580,10 @@
         <v>27</v>
       </c>
       <c r="B28" s="11" t="s">
-        <v>97</v>
+        <v>94</v>
       </c>
       <c r="C28" s="11" t="s">
-        <v>97</v>
+        <v>94</v>
       </c>
       <c r="D28" s="13">
         <v>0.67273088967606098</v>
@@ -3592,13 +3592,13 @@
         <v>31.889259854016199</v>
       </c>
       <c r="F28" s="10" t="s">
-        <v>72</v>
+        <v>70</v>
       </c>
       <c r="G28" s="11" t="s">
         <v>22</v>
       </c>
       <c r="H28" s="12" t="s">
-        <v>98</v>
+        <v>95</v>
       </c>
       <c r="I28" s="15">
         <v>1</v>
@@ -3622,10 +3622,10 @@
         <v>28</v>
       </c>
       <c r="B29" s="11" t="s">
-        <v>99</v>
+        <v>96</v>
       </c>
       <c r="C29" s="12" t="s">
-        <v>100</v>
+        <v>97</v>
       </c>
       <c r="D29" s="13">
         <v>0.64834354923902704</v>
@@ -3634,13 +3634,13 @@
         <v>31.918364767640298</v>
       </c>
       <c r="F29" s="10" t="s">
-        <v>72</v>
+        <v>70</v>
       </c>
       <c r="G29" s="11" t="s">
         <v>22</v>
       </c>
       <c r="H29" s="12" t="s">
-        <v>101</v>
+        <v>98</v>
       </c>
       <c r="I29" s="15">
         <v>1</v>
@@ -3664,10 +3664,10 @@
         <v>29</v>
       </c>
       <c r="B30" s="11" t="s">
-        <v>102</v>
+        <v>99</v>
       </c>
       <c r="C30" s="11" t="s">
-        <v>102</v>
+        <v>99</v>
       </c>
       <c r="D30" s="13">
         <v>0.232074758649122</v>
@@ -3676,13 +3676,13 @@
         <v>42.4753218118109</v>
       </c>
       <c r="F30" s="10" t="s">
-        <v>103</v>
+        <v>100</v>
       </c>
       <c r="G30" s="11" t="s">
         <v>17</v>
       </c>
       <c r="H30" s="12" t="s">
-        <v>104</v>
+        <v>637</v>
       </c>
       <c r="I30" s="15">
         <v>1</v>
@@ -3708,10 +3708,10 @@
         <v>30</v>
       </c>
       <c r="B31" s="11" t="s">
-        <v>105</v>
+        <v>101</v>
       </c>
       <c r="C31" s="11" t="s">
-        <v>105</v>
+        <v>101</v>
       </c>
       <c r="D31" s="13">
         <v>0.501006036217303</v>
@@ -3720,13 +3720,13 @@
         <v>29.9151053659204</v>
       </c>
       <c r="F31" s="10" t="s">
-        <v>106</v>
+        <v>102</v>
       </c>
       <c r="G31" s="11" t="s">
         <v>22</v>
       </c>
       <c r="H31" s="12" t="s">
-        <v>107</v>
+        <v>103</v>
       </c>
       <c r="I31" s="15">
         <v>1</v>
@@ -3750,10 +3750,10 @@
         <v>31</v>
       </c>
       <c r="B32" s="11" t="s">
-        <v>108</v>
+        <v>104</v>
       </c>
       <c r="C32" s="12" t="s">
-        <v>109</v>
+        <v>105</v>
       </c>
       <c r="D32" s="13">
         <v>0.888841648462812</v>
@@ -3762,19 +3762,19 @@
         <v>8.5324765936967406</v>
       </c>
       <c r="F32" s="10" t="s">
-        <v>110</v>
+        <v>106</v>
       </c>
       <c r="G32" s="11" t="s">
-        <v>42</v>
+        <v>41</v>
       </c>
       <c r="H32" s="12" t="s">
-        <v>111</v>
+        <v>632</v>
       </c>
       <c r="I32" s="17">
         <v>6.8000000000000005E-2</v>
       </c>
       <c r="J32" s="16" t="s">
-        <v>112</v>
+        <v>107</v>
       </c>
       <c r="K32" s="11">
         <v>3</v>
@@ -3789,7 +3789,7 @@
         <v>0</v>
       </c>
       <c r="O32" s="18" t="s">
-        <v>113</v>
+        <v>108</v>
       </c>
     </row>
     <row r="33" spans="1:15" x14ac:dyDescent="0.2">
@@ -3797,10 +3797,10 @@
         <v>32</v>
       </c>
       <c r="B33" s="11" t="s">
-        <v>114</v>
+        <v>109</v>
       </c>
       <c r="C33" s="11" t="s">
-        <v>114</v>
+        <v>109</v>
       </c>
       <c r="D33" s="13">
         <v>0.66795361364867001</v>
@@ -3809,13 +3809,13 @@
         <v>9.0055071922784808</v>
       </c>
       <c r="F33" s="10" t="s">
-        <v>110</v>
+        <v>106</v>
       </c>
       <c r="G33" s="11" t="s">
         <v>22</v>
       </c>
       <c r="H33" s="12" t="s">
-        <v>115</v>
+        <v>110</v>
       </c>
       <c r="I33" s="15">
         <v>0.96199999999999997</v>
@@ -3839,10 +3839,10 @@
         <v>33</v>
       </c>
       <c r="B34" s="11" t="s">
-        <v>116</v>
+        <v>111</v>
       </c>
       <c r="C34" s="12" t="s">
-        <v>117</v>
+        <v>112</v>
       </c>
       <c r="D34" s="13">
         <v>0.70080365864488003</v>
@@ -3851,13 +3851,13 @@
         <v>10.8564036576989</v>
       </c>
       <c r="F34" s="10" t="s">
-        <v>45</v>
+        <v>44</v>
       </c>
       <c r="G34" s="11" t="s">
         <v>22</v>
       </c>
       <c r="H34" s="12" t="s">
-        <v>118</v>
+        <v>113</v>
       </c>
       <c r="I34" s="17">
         <v>0.97099999999999997</v>
@@ -3878,7 +3878,7 @@
         <v>0</v>
       </c>
       <c r="O34" s="18" t="s">
-        <v>119</v>
+        <v>114</v>
       </c>
     </row>
     <row r="35" spans="1:15" x14ac:dyDescent="0.2">
@@ -3886,10 +3886,10 @@
         <v>34</v>
       </c>
       <c r="B35" s="11" t="s">
-        <v>120</v>
+        <v>115</v>
       </c>
       <c r="C35" s="12" t="s">
-        <v>121</v>
+        <v>116</v>
       </c>
       <c r="D35" s="13">
         <v>0.494461877195216</v>
@@ -3898,13 +3898,13 @@
         <v>13.637101812596701</v>
       </c>
       <c r="F35" s="10" t="s">
-        <v>122</v>
+        <v>117</v>
       </c>
       <c r="G35" s="11" t="s">
         <v>22</v>
       </c>
       <c r="H35" s="12" t="s">
-        <v>123</v>
+        <v>118</v>
       </c>
       <c r="I35" s="17">
         <v>0.98</v>
@@ -3925,7 +3925,7 @@
         <v>0</v>
       </c>
       <c r="O35" s="18" t="s">
-        <v>124</v>
+        <v>119</v>
       </c>
     </row>
     <row r="36" spans="1:15" x14ac:dyDescent="0.2">
@@ -3933,10 +3933,10 @@
         <v>35</v>
       </c>
       <c r="B36" s="11" t="s">
-        <v>125</v>
+        <v>120</v>
       </c>
       <c r="C36" s="11" t="s">
-        <v>125</v>
+        <v>120</v>
       </c>
       <c r="D36" s="13">
         <v>0.81257539729580797</v>
@@ -3945,13 +3945,13 @@
         <v>8.3305214862009809</v>
       </c>
       <c r="F36" s="10" t="s">
-        <v>51</v>
+        <v>49</v>
       </c>
       <c r="G36" s="11" t="s">
         <v>22</v>
       </c>
       <c r="H36" s="12" t="s">
-        <v>126</v>
+        <v>121</v>
       </c>
       <c r="I36" s="15">
         <v>0.95299999999999996</v>
@@ -3975,10 +3975,10 @@
         <v>36</v>
       </c>
       <c r="B37" s="11" t="s">
-        <v>127</v>
+        <v>122</v>
       </c>
       <c r="C37" s="12" t="s">
-        <v>128</v>
+        <v>123</v>
       </c>
       <c r="D37" s="13">
         <v>0.85137833775965999</v>
@@ -3987,13 +3987,13 @@
         <v>-0.67873255794174103</v>
       </c>
       <c r="F37" s="10" t="s">
-        <v>129</v>
+        <v>124</v>
       </c>
       <c r="G37" s="11" t="s">
         <v>22</v>
       </c>
       <c r="H37" s="12" t="s">
-        <v>130</v>
+        <v>125</v>
       </c>
       <c r="I37" s="15">
         <v>0.82399999999999995</v>
@@ -4017,10 +4017,10 @@
         <v>37</v>
       </c>
       <c r="B38" s="11" t="s">
-        <v>131</v>
+        <v>126</v>
       </c>
       <c r="C38" s="11" t="s">
-        <v>131</v>
+        <v>126</v>
       </c>
       <c r="D38" s="13">
         <v>0.839460055416128</v>
@@ -4029,13 +4029,13 @@
         <v>1.0281835501490399</v>
       </c>
       <c r="F38" s="10" t="s">
-        <v>132</v>
+        <v>127</v>
       </c>
       <c r="G38" s="11" t="s">
         <v>22</v>
       </c>
       <c r="H38" s="12" t="s">
-        <v>133</v>
+        <v>128</v>
       </c>
       <c r="I38" s="15">
         <v>0.85899999999999999</v>
@@ -4059,10 +4059,10 @@
         <v>38</v>
       </c>
       <c r="B39" s="11" t="s">
-        <v>134</v>
+        <v>129</v>
       </c>
       <c r="C39" s="11" t="s">
-        <v>134</v>
+        <v>129</v>
       </c>
       <c r="D39" s="13">
         <v>0.73128039139643797</v>
@@ -4071,13 +4071,13 @@
         <v>7.1116933053247902</v>
       </c>
       <c r="F39" s="10" t="s">
-        <v>135</v>
+        <v>130</v>
       </c>
       <c r="G39" s="11" t="s">
         <v>22</v>
       </c>
       <c r="H39" s="12" t="s">
-        <v>136</v>
+        <v>131</v>
       </c>
       <c r="I39" s="15">
         <v>1</v>
@@ -4101,10 +4101,10 @@
         <v>39</v>
       </c>
       <c r="B40" s="11" t="s">
-        <v>137</v>
+        <v>132</v>
       </c>
       <c r="C40" s="11" t="s">
-        <v>137</v>
+        <v>132</v>
       </c>
       <c r="D40" s="13">
         <v>0.90344737272875997</v>
@@ -4119,7 +4119,7 @@
         <v>22</v>
       </c>
       <c r="H40" s="12" t="s">
-        <v>138</v>
+        <v>133</v>
       </c>
       <c r="I40" s="15">
         <v>0.89700000000000002</v>
@@ -4143,10 +4143,10 @@
         <v>40</v>
       </c>
       <c r="B41" s="11" t="s">
-        <v>139</v>
+        <v>134</v>
       </c>
       <c r="C41" s="11" t="s">
-        <v>139</v>
+        <v>134</v>
       </c>
       <c r="D41" s="13">
         <v>0.84110376774554196</v>
@@ -4155,19 +4155,19 @@
         <v>12.2987157179472</v>
       </c>
       <c r="F41" s="10" t="s">
-        <v>63</v>
+        <v>61</v>
       </c>
       <c r="G41" s="11" t="s">
         <v>22</v>
       </c>
       <c r="H41" s="12" t="s">
-        <v>140</v>
+        <v>135</v>
       </c>
       <c r="I41" s="15">
         <v>0.97899999999999998</v>
       </c>
       <c r="J41" s="16" t="s">
-        <v>112</v>
+        <v>107</v>
       </c>
       <c r="K41" s="11">
         <v>3</v>
@@ -4215,7 +4215,7 @@
   <sheetData>
     <row r="1" spans="1:5" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A1" s="19" t="s">
-        <v>141</v>
+        <v>136</v>
       </c>
       <c r="B1" s="20">
         <f>COUNTIF(Districts!G:G,"=No_Incumbent")</f>
@@ -4232,7 +4232,7 @@
     </row>
     <row r="2" spans="1:5" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A2" s="19" t="s">
-        <v>142</v>
+        <v>137</v>
       </c>
       <c r="B2" s="20">
         <f>COUNTIF(Districts!L:L, "&gt;1")+COUNTIF(Districts!M:M, "&gt;1")</f>
@@ -4245,7 +4245,7 @@
     </row>
     <row r="3" spans="1:5" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A3" s="19" t="s">
-        <v>143</v>
+        <v>138</v>
       </c>
       <c r="B3" s="20">
         <f>COUNTIF(Districts!K:K,"&gt;1")</f>
@@ -4258,7 +4258,7 @@
     </row>
     <row r="4" spans="1:5" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A4" s="19" t="s">
-        <v>144</v>
+        <v>139</v>
       </c>
       <c r="B4" s="20">
         <f>COUNTIF(Districts!K:K,"=1")</f>
@@ -4271,7 +4271,7 @@
     </row>
     <row r="5" spans="1:5" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A5" s="19" t="s">
-        <v>145</v>
+        <v>140</v>
       </c>
       <c r="B5" s="20">
         <f>COUNTIF(Districts!G:G, "Dem_Incumbent")</f>
@@ -4281,7 +4281,7 @@
     </row>
     <row r="6" spans="1:5" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A6" s="19" t="s">
-        <v>146</v>
+        <v>141</v>
       </c>
       <c r="B6" s="20">
         <f>COUNTIF(Districts!G:G, "GOP_Incumbent")</f>
@@ -4291,7 +4291,7 @@
     </row>
     <row r="7" spans="1:5" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A7" s="19" t="s">
-        <v>147</v>
+        <v>142</v>
       </c>
       <c r="B7" s="20">
         <f ca="1">IFERROR(__xludf.DUMMYFUNCTION("INDEX(QUERY(Districts!$G:$N, ""select count(G) where G='Dem_Incumbent' and K&gt;1""),2)"),17)</f>
@@ -4304,7 +4304,7 @@
     </row>
     <row r="8" spans="1:5" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A8" s="19" t="s">
-        <v>148</v>
+        <v>143</v>
       </c>
       <c r="B8" s="20" t="str">
         <f ca="1">IFERROR(__xludf.DUMMYFUNCTION("INDEX(QUERY(Districts!$G:$N, ""select count(G) where G='GOP_Incumbent' and L&gt;1""),2)"),"#REF!")</f>
@@ -4317,7 +4317,7 @@
     </row>
     <row r="9" spans="1:5" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A9" s="19" t="s">
-        <v>149</v>
+        <v>144</v>
       </c>
       <c r="B9" s="20">
         <f ca="1">IFERROR(__xludf.DUMMYFUNCTION("INDEX(QUERY(Districts!$G:$N, ""select count(G) where G='Dem_Incumbent' and ((L&gt;0)or(M&gt;0))""),2)"),32)</f>
@@ -4328,9 +4328,9 @@
         <v>1</v>
       </c>
     </row>
-    <row r="10" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="10" spans="1:5" ht="13" x14ac:dyDescent="0.15">
       <c r="A10" s="19" t="s">
-        <v>150</v>
+        <v>145</v>
       </c>
       <c r="B10" s="22">
         <f ca="1">IFERROR(__xludf.DUMMYFUNCTION("INDEX(QUERY(Districts!$G:$N, ""select count(G) where G='GOP_Incumbent' and ((K&gt;0)or(M&gt;0))""),2)"),3)</f>
@@ -4343,7 +4343,7 @@
     </row>
     <row r="11" spans="1:5" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A11" s="19" t="s">
-        <v>151</v>
+        <v>146</v>
       </c>
       <c r="B11" s="20">
         <f>COUNTIFS(Districts!G:G,"=Dem_Incumbent", Districts!K:K,"=1")</f>
@@ -4356,7 +4356,7 @@
     </row>
     <row r="12" spans="1:5" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A12" s="19" t="s">
-        <v>152</v>
+        <v>147</v>
       </c>
       <c r="B12" s="20">
         <f>COUNTIFS(Districts!G:G,"=GOP_Incumbent", Districts!K:K,"=1")</f>
@@ -8379,37 +8379,37 @@
   <sheetData>
     <row r="1" spans="1:25" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A1" s="1" t="s">
-        <v>153</v>
+        <v>148</v>
       </c>
       <c r="B1" s="3" t="s">
         <v>1</v>
       </c>
       <c r="C1" s="8" t="s">
-        <v>154</v>
+        <v>149</v>
       </c>
       <c r="D1" s="3" t="s">
         <v>7</v>
       </c>
       <c r="E1" s="3" t="s">
+        <v>150</v>
+      </c>
+      <c r="F1" s="3" t="s">
+        <v>151</v>
+      </c>
+      <c r="G1" s="3" t="s">
+        <v>152</v>
+      </c>
+      <c r="H1" s="3" t="s">
+        <v>153</v>
+      </c>
+      <c r="I1" s="1" t="s">
+        <v>154</v>
+      </c>
+      <c r="J1" s="3" t="s">
         <v>155</v>
       </c>
-      <c r="F1" s="3" t="s">
+      <c r="K1" s="3" t="s">
         <v>156</v>
-      </c>
-      <c r="G1" s="3" t="s">
-        <v>157</v>
-      </c>
-      <c r="H1" s="3" t="s">
-        <v>158</v>
-      </c>
-      <c r="I1" s="1" t="s">
-        <v>159</v>
-      </c>
-      <c r="J1" s="3" t="s">
-        <v>160</v>
-      </c>
-      <c r="K1" s="3" t="s">
-        <v>161</v>
       </c>
       <c r="L1" s="9"/>
       <c r="M1" s="9"/>
@@ -8428,42 +8428,42 @@
     </row>
     <row r="2" spans="1:25" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A2" s="24" t="s">
-        <v>162</v>
+        <v>157</v>
       </c>
       <c r="B2" s="12" t="s">
         <v>14</v>
       </c>
       <c r="C2" s="25" t="s">
-        <v>163</v>
+        <v>158</v>
       </c>
       <c r="D2" s="12" t="s">
-        <v>164</v>
+        <v>159</v>
       </c>
       <c r="E2" s="12" t="s">
-        <v>165</v>
+        <v>160</v>
       </c>
       <c r="F2" s="12" t="s">
         <v>18</v>
       </c>
       <c r="G2" s="12" t="s">
-        <v>166</v>
+        <v>161</v>
       </c>
       <c r="H2" s="26" t="s">
-        <v>167</v>
+        <v>162</v>
       </c>
       <c r="I2" s="24" t="s">
-        <v>168</v>
+        <v>163</v>
       </c>
       <c r="J2" s="12" t="s">
-        <v>169</v>
+        <v>164</v>
       </c>
       <c r="K2" s="27" t="s">
-        <v>170</v>
+        <v>165</v>
       </c>
     </row>
     <row r="3" spans="1:25" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A3" s="24" t="s">
-        <v>162</v>
+        <v>157</v>
       </c>
       <c r="B3" s="12" t="s">
         <v>14</v>
@@ -8472,95 +8472,95 @@
         <v>18113</v>
       </c>
       <c r="D3" s="12" t="s">
-        <v>164</v>
+        <v>159</v>
       </c>
       <c r="E3" s="12" t="s">
-        <v>171</v>
+        <v>166</v>
       </c>
       <c r="F3" s="12" t="s">
         <v>18</v>
       </c>
       <c r="G3" s="12" t="s">
-        <v>172</v>
+        <v>167</v>
       </c>
       <c r="H3" s="26" t="s">
-        <v>173</v>
+        <v>168</v>
       </c>
       <c r="I3" s="29">
         <v>44718</v>
       </c>
       <c r="J3" s="12" t="s">
-        <v>174</v>
+        <v>169</v>
       </c>
     </row>
     <row r="4" spans="1:25" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A4" s="24" t="s">
-        <v>162</v>
+        <v>157</v>
       </c>
       <c r="B4" s="12" t="s">
         <v>14</v>
       </c>
       <c r="C4" s="25" t="s">
+        <v>170</v>
+      </c>
+      <c r="D4" s="12" t="s">
+        <v>159</v>
+      </c>
+      <c r="E4" s="12" t="s">
+        <v>171</v>
+      </c>
+      <c r="F4" s="12" t="s">
+        <v>172</v>
+      </c>
+      <c r="G4" s="12" t="s">
+        <v>173</v>
+      </c>
+      <c r="H4" s="26" t="s">
+        <v>174</v>
+      </c>
+      <c r="I4" s="24" t="s">
         <v>175</v>
       </c>
-      <c r="D4" s="12" t="s">
-        <v>164</v>
-      </c>
-      <c r="E4" s="12" t="s">
+      <c r="J4" s="12" t="s">
         <v>176</v>
       </c>
-      <c r="F4" s="12" t="s">
+      <c r="K4" s="27" t="s">
         <v>177</v>
-      </c>
-      <c r="G4" s="12" t="s">
-        <v>178</v>
-      </c>
-      <c r="H4" s="26" t="s">
-        <v>179</v>
-      </c>
-      <c r="I4" s="24" t="s">
-        <v>180</v>
-      </c>
-      <c r="J4" s="12" t="s">
-        <v>181</v>
-      </c>
-      <c r="K4" s="27" t="s">
-        <v>182</v>
       </c>
     </row>
     <row r="5" spans="1:25" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A5" s="30" t="s">
-        <v>183</v>
+        <v>178</v>
       </c>
       <c r="B5" s="31" t="s">
         <v>19</v>
       </c>
       <c r="C5" s="32" t="s">
-        <v>184</v>
+        <v>179</v>
       </c>
       <c r="D5" s="31" t="s">
-        <v>185</v>
+        <v>180</v>
       </c>
       <c r="E5" s="33" t="s">
-        <v>186</v>
+        <v>181</v>
       </c>
       <c r="F5" s="31" t="s">
         <v>18</v>
       </c>
       <c r="G5" s="31" t="s">
-        <v>187</v>
+        <v>182</v>
       </c>
       <c r="H5" s="31" t="s">
-        <v>188</v>
+        <v>183</v>
       </c>
       <c r="I5" s="30" t="s">
-        <v>189</v>
+        <v>184</v>
       </c>
       <c r="J5" s="31" t="s">
-        <v>190</v>
+        <v>185</v>
       </c>
       <c r="K5" s="34" t="s">
-        <v>191</v>
+        <v>186</v>
       </c>
       <c r="L5" s="35"/>
       <c r="M5" s="35"/>
@@ -8579,37 +8579,37 @@
     </row>
     <row r="6" spans="1:25" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A6" s="30" t="s">
-        <v>183</v>
+        <v>178</v>
       </c>
       <c r="B6" s="31" t="s">
         <v>19</v>
       </c>
       <c r="C6" s="32" t="s">
+        <v>187</v>
+      </c>
+      <c r="D6" s="31" t="s">
+        <v>159</v>
+      </c>
+      <c r="E6" s="31" t="s">
+        <v>188</v>
+      </c>
+      <c r="F6" s="31" t="s">
+        <v>107</v>
+      </c>
+      <c r="G6" s="31" t="s">
+        <v>189</v>
+      </c>
+      <c r="H6" s="36" t="s">
+        <v>190</v>
+      </c>
+      <c r="I6" s="30" t="s">
+        <v>191</v>
+      </c>
+      <c r="J6" s="31" t="s">
         <v>192</v>
       </c>
-      <c r="D6" s="31" t="s">
-        <v>164</v>
-      </c>
-      <c r="E6" s="31" t="s">
+      <c r="K6" s="34" t="s">
         <v>193</v>
-      </c>
-      <c r="F6" s="31" t="s">
-        <v>112</v>
-      </c>
-      <c r="G6" s="31" t="s">
-        <v>194</v>
-      </c>
-      <c r="H6" s="36" t="s">
-        <v>195</v>
-      </c>
-      <c r="I6" s="30" t="s">
-        <v>196</v>
-      </c>
-      <c r="J6" s="31" t="s">
-        <v>197</v>
-      </c>
-      <c r="K6" s="34" t="s">
-        <v>198</v>
       </c>
       <c r="L6" s="35"/>
       <c r="M6" s="35"/>
@@ -8628,174 +8628,174 @@
     </row>
     <row r="7" spans="1:25" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A7" s="24" t="s">
-        <v>199</v>
+        <v>194</v>
       </c>
       <c r="B7" s="12" t="s">
         <v>27</v>
       </c>
       <c r="C7" s="25" t="s">
-        <v>200</v>
+        <v>195</v>
       </c>
       <c r="D7" s="12" t="s">
-        <v>164</v>
+        <v>159</v>
       </c>
       <c r="E7" s="12" t="s">
-        <v>201</v>
+        <v>196</v>
       </c>
       <c r="F7" s="12" t="s">
         <v>18</v>
       </c>
       <c r="G7" s="12" t="s">
-        <v>202</v>
+        <v>197</v>
       </c>
       <c r="H7" s="26" t="s">
-        <v>203</v>
+        <v>198</v>
       </c>
       <c r="I7" s="24" t="s">
-        <v>204</v>
+        <v>199</v>
       </c>
       <c r="J7" s="12" t="s">
-        <v>205</v>
+        <v>200</v>
       </c>
       <c r="K7" s="27" t="s">
-        <v>206</v>
+        <v>201</v>
       </c>
     </row>
     <row r="8" spans="1:25" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A8" s="24" t="s">
-        <v>199</v>
+        <v>194</v>
       </c>
       <c r="B8" s="12" t="s">
         <v>27</v>
       </c>
       <c r="C8" s="25" t="s">
-        <v>207</v>
+        <v>202</v>
       </c>
       <c r="D8" s="12" t="s">
-        <v>164</v>
+        <v>159</v>
       </c>
       <c r="E8" s="12" t="s">
-        <v>208</v>
+        <v>203</v>
       </c>
       <c r="F8" s="12" t="s">
         <v>18</v>
       </c>
       <c r="G8" s="12" t="s">
-        <v>209</v>
+        <v>204</v>
       </c>
       <c r="H8" s="26" t="s">
-        <v>210</v>
+        <v>205</v>
       </c>
       <c r="I8" s="24" t="s">
-        <v>211</v>
+        <v>206</v>
       </c>
       <c r="J8" s="12" t="s">
-        <v>212</v>
+        <v>207</v>
       </c>
       <c r="K8" s="27" t="s">
-        <v>213</v>
+        <v>208</v>
       </c>
     </row>
     <row r="9" spans="1:25" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A9" s="24" t="s">
-        <v>199</v>
+        <v>194</v>
       </c>
       <c r="B9" s="12" t="s">
         <v>27</v>
       </c>
       <c r="C9" s="25" t="s">
+        <v>209</v>
+      </c>
+      <c r="D9" s="12" t="s">
+        <v>159</v>
+      </c>
+      <c r="E9" s="12" t="s">
+        <v>210</v>
+      </c>
+      <c r="F9" s="12" t="s">
+        <v>107</v>
+      </c>
+      <c r="G9" s="12" t="s">
+        <v>211</v>
+      </c>
+      <c r="H9" s="26" t="s">
+        <v>212</v>
+      </c>
+      <c r="I9" s="24" t="s">
+        <v>213</v>
+      </c>
+      <c r="J9" s="12" t="s">
         <v>214</v>
       </c>
-      <c r="D9" s="12" t="s">
-        <v>164</v>
-      </c>
-      <c r="E9" s="12" t="s">
+      <c r="K9" s="27" t="s">
         <v>215</v>
-      </c>
-      <c r="F9" s="12" t="s">
-        <v>112</v>
-      </c>
-      <c r="G9" s="12" t="s">
-        <v>216</v>
-      </c>
-      <c r="H9" s="26" t="s">
-        <v>217</v>
-      </c>
-      <c r="I9" s="24" t="s">
-        <v>218</v>
-      </c>
-      <c r="J9" s="12" t="s">
-        <v>219</v>
-      </c>
-      <c r="K9" s="27" t="s">
-        <v>220</v>
       </c>
     </row>
     <row r="10" spans="1:25" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A10" s="24" t="s">
-        <v>199</v>
+        <v>194</v>
       </c>
       <c r="B10" s="12" t="s">
         <v>27</v>
       </c>
       <c r="C10" s="25" t="s">
+        <v>216</v>
+      </c>
+      <c r="D10" s="12" t="s">
+        <v>159</v>
+      </c>
+      <c r="E10" s="12" t="s">
+        <v>217</v>
+      </c>
+      <c r="F10" s="12" t="s">
+        <v>107</v>
+      </c>
+      <c r="G10" s="12" t="s">
+        <v>218</v>
+      </c>
+      <c r="H10" s="26" t="s">
+        <v>219</v>
+      </c>
+      <c r="I10" s="24" t="s">
+        <v>220</v>
+      </c>
+      <c r="J10" s="12" t="s">
         <v>221</v>
-      </c>
-      <c r="D10" s="12" t="s">
-        <v>164</v>
-      </c>
-      <c r="E10" s="12" t="s">
-        <v>222</v>
-      </c>
-      <c r="F10" s="12" t="s">
-        <v>112</v>
-      </c>
-      <c r="G10" s="12" t="s">
-        <v>223</v>
-      </c>
-      <c r="H10" s="26" t="s">
-        <v>224</v>
-      </c>
-      <c r="I10" s="24" t="s">
-        <v>225</v>
-      </c>
-      <c r="J10" s="12" t="s">
-        <v>226</v>
       </c>
     </row>
     <row r="11" spans="1:25" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A11" s="30" t="s">
-        <v>227</v>
+        <v>222</v>
       </c>
       <c r="B11" s="31" t="s">
-        <v>35</v>
+        <v>34</v>
       </c>
       <c r="C11" s="32" t="s">
-        <v>228</v>
+        <v>223</v>
       </c>
       <c r="D11" s="31" t="s">
-        <v>185</v>
+        <v>180</v>
       </c>
       <c r="E11" s="33" t="s">
-        <v>229</v>
+        <v>224</v>
       </c>
       <c r="F11" s="31" t="s">
         <v>18</v>
       </c>
       <c r="G11" s="31" t="s">
-        <v>230</v>
+        <v>225</v>
       </c>
       <c r="H11" s="36" t="s">
-        <v>231</v>
+        <v>226</v>
       </c>
       <c r="I11" s="30" t="s">
-        <v>232</v>
+        <v>227</v>
       </c>
       <c r="J11" s="31" t="s">
-        <v>190</v>
+        <v>185</v>
       </c>
       <c r="K11" s="34" t="s">
-        <v>233</v>
+        <v>228</v>
       </c>
       <c r="L11" s="35"/>
       <c r="M11" s="35"/>
@@ -8814,37 +8814,37 @@
     </row>
     <row r="12" spans="1:25" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A12" s="30" t="s">
-        <v>227</v>
+        <v>222</v>
       </c>
       <c r="B12" s="31" t="s">
-        <v>35</v>
+        <v>34</v>
       </c>
       <c r="C12" s="32" t="s">
+        <v>229</v>
+      </c>
+      <c r="D12" s="31" t="s">
+        <v>159</v>
+      </c>
+      <c r="E12" s="31" t="s">
+        <v>230</v>
+      </c>
+      <c r="F12" s="31" t="s">
+        <v>107</v>
+      </c>
+      <c r="G12" s="31" t="s">
+        <v>231</v>
+      </c>
+      <c r="H12" s="36" t="s">
+        <v>232</v>
+      </c>
+      <c r="I12" s="30" t="s">
+        <v>233</v>
+      </c>
+      <c r="J12" s="31" t="s">
         <v>234</v>
       </c>
-      <c r="D12" s="31" t="s">
-        <v>164</v>
-      </c>
-      <c r="E12" s="31" t="s">
+      <c r="K12" s="34" t="s">
         <v>235</v>
-      </c>
-      <c r="F12" s="31" t="s">
-        <v>112</v>
-      </c>
-      <c r="G12" s="31" t="s">
-        <v>236</v>
-      </c>
-      <c r="H12" s="36" t="s">
-        <v>237</v>
-      </c>
-      <c r="I12" s="30" t="s">
-        <v>238</v>
-      </c>
-      <c r="J12" s="31" t="s">
-        <v>239</v>
-      </c>
-      <c r="K12" s="34" t="s">
-        <v>240</v>
       </c>
       <c r="L12" s="35"/>
       <c r="M12" s="35"/>
@@ -8863,139 +8863,139 @@
     </row>
     <row r="13" spans="1:25" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A13" s="24" t="s">
-        <v>241</v>
+        <v>236</v>
       </c>
       <c r="B13" s="12" t="s">
-        <v>47</v>
+        <v>46</v>
       </c>
       <c r="C13" s="25" t="s">
-        <v>242</v>
+        <v>237</v>
       </c>
       <c r="D13" s="12" t="s">
-        <v>164</v>
+        <v>159</v>
       </c>
       <c r="E13" s="12" t="s">
-        <v>243</v>
+        <v>238</v>
       </c>
       <c r="F13" s="12" t="s">
         <v>18</v>
       </c>
       <c r="G13" s="12" t="s">
-        <v>244</v>
+        <v>239</v>
       </c>
       <c r="H13" s="26" t="s">
-        <v>245</v>
+        <v>240</v>
       </c>
       <c r="I13" s="24" t="s">
-        <v>246</v>
+        <v>241</v>
       </c>
       <c r="J13" s="12" t="s">
-        <v>247</v>
+        <v>242</v>
       </c>
       <c r="K13" s="27" t="s">
-        <v>248</v>
+        <v>243</v>
       </c>
     </row>
     <row r="14" spans="1:25" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A14" s="24" t="s">
-        <v>241</v>
+        <v>236</v>
       </c>
       <c r="B14" s="12" t="s">
-        <v>47</v>
+        <v>46</v>
       </c>
       <c r="C14" s="25" t="s">
-        <v>249</v>
+        <v>244</v>
       </c>
       <c r="D14" s="12" t="s">
-        <v>164</v>
+        <v>159</v>
       </c>
       <c r="E14" s="12" t="s">
-        <v>250</v>
+        <v>245</v>
       </c>
       <c r="F14" s="12" t="s">
         <v>18</v>
       </c>
       <c r="G14" s="12" t="s">
-        <v>244</v>
+        <v>239</v>
       </c>
       <c r="H14" s="26" t="s">
-        <v>251</v>
+        <v>246</v>
       </c>
       <c r="I14" s="24" t="s">
-        <v>252</v>
+        <v>247</v>
       </c>
       <c r="J14" s="12" t="s">
-        <v>253</v>
+        <v>248</v>
       </c>
       <c r="K14" s="27" t="s">
-        <v>254</v>
+        <v>249</v>
       </c>
     </row>
     <row r="15" spans="1:25" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A15" s="24" t="s">
-        <v>241</v>
+        <v>236</v>
       </c>
       <c r="B15" s="12" t="s">
-        <v>47</v>
+        <v>46</v>
       </c>
       <c r="C15" s="25" t="s">
+        <v>250</v>
+      </c>
+      <c r="D15" s="12" t="s">
+        <v>159</v>
+      </c>
+      <c r="E15" s="12" t="s">
+        <v>251</v>
+      </c>
+      <c r="F15" s="12" t="s">
+        <v>172</v>
+      </c>
+      <c r="G15" s="12" t="s">
+        <v>252</v>
+      </c>
+      <c r="H15" s="26" t="s">
+        <v>253</v>
+      </c>
+      <c r="I15" s="24" t="s">
+        <v>254</v>
+      </c>
+      <c r="J15" s="12" t="s">
         <v>255</v>
-      </c>
-      <c r="D15" s="12" t="s">
-        <v>164</v>
-      </c>
-      <c r="E15" s="12" t="s">
-        <v>256</v>
-      </c>
-      <c r="F15" s="12" t="s">
-        <v>177</v>
-      </c>
-      <c r="G15" s="12" t="s">
-        <v>257</v>
-      </c>
-      <c r="H15" s="26" t="s">
-        <v>258</v>
-      </c>
-      <c r="I15" s="24" t="s">
-        <v>259</v>
-      </c>
-      <c r="J15" s="12" t="s">
-        <v>260</v>
       </c>
     </row>
     <row r="16" spans="1:25" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A16" s="30" t="s">
-        <v>261</v>
+        <v>256</v>
       </c>
       <c r="B16" s="31" t="s">
-        <v>50</v>
+        <v>48</v>
       </c>
       <c r="C16" s="32" t="s">
-        <v>262</v>
+        <v>257</v>
       </c>
       <c r="D16" s="31" t="s">
-        <v>185</v>
+        <v>180</v>
       </c>
       <c r="E16" s="33" t="s">
-        <v>263</v>
+        <v>258</v>
       </c>
       <c r="F16" s="31" t="s">
         <v>18</v>
       </c>
       <c r="G16" s="31" t="s">
-        <v>264</v>
+        <v>259</v>
       </c>
       <c r="H16" s="36" t="s">
-        <v>265</v>
+        <v>260</v>
       </c>
       <c r="I16" s="30" t="s">
-        <v>266</v>
+        <v>261</v>
       </c>
       <c r="J16" s="31" t="s">
-        <v>267</v>
+        <v>262</v>
       </c>
       <c r="K16" s="34" t="s">
-        <v>268</v>
+        <v>263</v>
       </c>
       <c r="L16" s="35"/>
       <c r="M16" s="35"/>
@@ -9014,34 +9014,34 @@
     </row>
     <row r="17" spans="1:25" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A17" s="30" t="s">
-        <v>261</v>
+        <v>256</v>
       </c>
       <c r="B17" s="31" t="s">
-        <v>50</v>
+        <v>48</v>
       </c>
       <c r="C17" s="32" t="s">
+        <v>264</v>
+      </c>
+      <c r="D17" s="31" t="s">
+        <v>159</v>
+      </c>
+      <c r="E17" s="31" t="s">
+        <v>265</v>
+      </c>
+      <c r="F17" s="31" t="s">
+        <v>107</v>
+      </c>
+      <c r="G17" s="31" t="s">
+        <v>266</v>
+      </c>
+      <c r="H17" s="36" t="s">
+        <v>267</v>
+      </c>
+      <c r="I17" s="30" t="s">
+        <v>268</v>
+      </c>
+      <c r="J17" s="31" t="s">
         <v>269</v>
-      </c>
-      <c r="D17" s="31" t="s">
-        <v>164</v>
-      </c>
-      <c r="E17" s="31" t="s">
-        <v>270</v>
-      </c>
-      <c r="F17" s="31" t="s">
-        <v>112</v>
-      </c>
-      <c r="G17" s="31" t="s">
-        <v>271</v>
-      </c>
-      <c r="H17" s="36" t="s">
-        <v>272</v>
-      </c>
-      <c r="I17" s="30" t="s">
-        <v>273</v>
-      </c>
-      <c r="J17" s="31" t="s">
-        <v>274</v>
       </c>
       <c r="K17" s="35"/>
       <c r="L17" s="35"/>
@@ -9061,104 +9061,104 @@
     </row>
     <row r="18" spans="1:25" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A18" s="24" t="s">
-        <v>275</v>
+        <v>270</v>
       </c>
       <c r="B18" s="12" t="s">
-        <v>55</v>
+        <v>53</v>
       </c>
       <c r="C18" s="25" t="s">
-        <v>276</v>
+        <v>271</v>
       </c>
       <c r="D18" s="12" t="s">
-        <v>185</v>
+        <v>180</v>
       </c>
       <c r="E18" s="3" t="s">
-        <v>277</v>
+        <v>272</v>
       </c>
       <c r="F18" s="12" t="s">
         <v>18</v>
       </c>
       <c r="G18" s="12" t="s">
-        <v>278</v>
+        <v>273</v>
       </c>
       <c r="H18" s="12" t="s">
-        <v>279</v>
+        <v>274</v>
       </c>
       <c r="I18" s="24" t="s">
-        <v>280</v>
+        <v>275</v>
       </c>
       <c r="J18" s="12" t="s">
-        <v>281</v>
+        <v>276</v>
       </c>
       <c r="K18" s="37" t="s">
-        <v>282</v>
+        <v>277</v>
       </c>
     </row>
     <row r="19" spans="1:25" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A19" s="24" t="s">
-        <v>275</v>
+        <v>270</v>
       </c>
       <c r="B19" s="12" t="s">
-        <v>55</v>
+        <v>53</v>
       </c>
       <c r="C19" s="25" t="s">
+        <v>278</v>
+      </c>
+      <c r="D19" s="12" t="s">
+        <v>159</v>
+      </c>
+      <c r="E19" s="12" t="s">
+        <v>279</v>
+      </c>
+      <c r="F19" s="12" t="s">
+        <v>107</v>
+      </c>
+      <c r="G19" s="12" t="s">
+        <v>280</v>
+      </c>
+      <c r="H19" s="26" t="s">
+        <v>281</v>
+      </c>
+      <c r="I19" s="24" t="s">
+        <v>282</v>
+      </c>
+      <c r="J19" s="12" t="s">
         <v>283</v>
-      </c>
-      <c r="D19" s="12" t="s">
-        <v>164</v>
-      </c>
-      <c r="E19" s="12" t="s">
-        <v>284</v>
-      </c>
-      <c r="F19" s="12" t="s">
-        <v>112</v>
-      </c>
-      <c r="G19" s="12" t="s">
-        <v>285</v>
-      </c>
-      <c r="H19" s="26" t="s">
-        <v>286</v>
-      </c>
-      <c r="I19" s="24" t="s">
-        <v>287</v>
-      </c>
-      <c r="J19" s="12" t="s">
-        <v>288</v>
       </c>
     </row>
     <row r="20" spans="1:25" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A20" s="30" t="s">
-        <v>289</v>
+        <v>284</v>
       </c>
       <c r="B20" s="31" t="s">
-        <v>61</v>
+        <v>59</v>
       </c>
       <c r="C20" s="32" t="s">
-        <v>290</v>
+        <v>285</v>
       </c>
       <c r="D20" s="31" t="s">
-        <v>185</v>
+        <v>180</v>
       </c>
       <c r="E20" s="33" t="s">
-        <v>291</v>
+        <v>286</v>
       </c>
       <c r="F20" s="31" t="s">
         <v>18</v>
       </c>
       <c r="G20" s="31" t="s">
-        <v>292</v>
+        <v>287</v>
       </c>
       <c r="H20" s="36" t="s">
-        <v>293</v>
+        <v>288</v>
       </c>
       <c r="I20" s="30" t="s">
-        <v>294</v>
+        <v>289</v>
       </c>
       <c r="J20" s="31" t="s">
-        <v>295</v>
+        <v>290</v>
       </c>
       <c r="K20" s="34" t="s">
-        <v>296</v>
+        <v>291</v>
       </c>
       <c r="L20" s="35"/>
       <c r="M20" s="35"/>
@@ -9177,37 +9177,37 @@
     </row>
     <row r="21" spans="1:25" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A21" s="30" t="s">
-        <v>289</v>
+        <v>284</v>
       </c>
       <c r="B21" s="31" t="s">
-        <v>61</v>
+        <v>59</v>
       </c>
       <c r="C21" s="32" t="s">
+        <v>292</v>
+      </c>
+      <c r="D21" s="31" t="s">
+        <v>159</v>
+      </c>
+      <c r="E21" s="31" t="s">
+        <v>293</v>
+      </c>
+      <c r="F21" s="31" t="s">
+        <v>107</v>
+      </c>
+      <c r="G21" s="31" t="s">
+        <v>294</v>
+      </c>
+      <c r="H21" s="36" t="s">
+        <v>295</v>
+      </c>
+      <c r="I21" s="30" t="s">
+        <v>296</v>
+      </c>
+      <c r="J21" s="31" t="s">
+        <v>164</v>
+      </c>
+      <c r="K21" s="34" t="s">
         <v>297</v>
-      </c>
-      <c r="D21" s="31" t="s">
-        <v>164</v>
-      </c>
-      <c r="E21" s="31" t="s">
-        <v>298</v>
-      </c>
-      <c r="F21" s="31" t="s">
-        <v>112</v>
-      </c>
-      <c r="G21" s="31" t="s">
-        <v>299</v>
-      </c>
-      <c r="H21" s="36" t="s">
-        <v>300</v>
-      </c>
-      <c r="I21" s="30" t="s">
-        <v>301</v>
-      </c>
-      <c r="J21" s="31" t="s">
-        <v>169</v>
-      </c>
-      <c r="K21" s="34" t="s">
-        <v>302</v>
       </c>
       <c r="L21" s="35"/>
       <c r="M21" s="35"/>
@@ -9226,142 +9226,142 @@
     </row>
     <row r="22" spans="1:25" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A22" s="24" t="s">
-        <v>303</v>
+        <v>298</v>
       </c>
       <c r="B22" s="12" t="s">
-        <v>76</v>
+        <v>74</v>
       </c>
       <c r="C22" s="25" t="s">
-        <v>304</v>
+        <v>299</v>
       </c>
       <c r="D22" s="12" t="s">
-        <v>164</v>
+        <v>159</v>
       </c>
       <c r="E22" s="12" t="s">
-        <v>305</v>
+        <v>300</v>
       </c>
       <c r="F22" s="12" t="s">
         <v>18</v>
       </c>
       <c r="G22" s="12" t="s">
-        <v>306</v>
+        <v>301</v>
       </c>
       <c r="H22" s="26" t="s">
-        <v>307</v>
+        <v>302</v>
       </c>
       <c r="I22" s="24" t="s">
-        <v>308</v>
+        <v>303</v>
       </c>
       <c r="J22" s="12" t="s">
-        <v>309</v>
+        <v>304</v>
       </c>
       <c r="K22" s="27" t="s">
-        <v>310</v>
+        <v>305</v>
       </c>
     </row>
     <row r="23" spans="1:25" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A23" s="24" t="s">
-        <v>303</v>
+        <v>298</v>
       </c>
       <c r="B23" s="12" t="s">
-        <v>76</v>
+        <v>74</v>
       </c>
       <c r="C23" s="25" t="s">
-        <v>311</v>
+        <v>306</v>
       </c>
       <c r="D23" s="12" t="s">
-        <v>164</v>
+        <v>159</v>
       </c>
       <c r="E23" s="12" t="s">
-        <v>312</v>
+        <v>307</v>
       </c>
       <c r="F23" s="12" t="s">
         <v>18</v>
       </c>
       <c r="G23" s="12" t="s">
-        <v>306</v>
+        <v>301</v>
       </c>
       <c r="H23" s="26" t="s">
-        <v>307</v>
+        <v>302</v>
       </c>
       <c r="I23" s="24" t="s">
-        <v>313</v>
+        <v>308</v>
       </c>
       <c r="J23" s="12" t="s">
-        <v>314</v>
+        <v>309</v>
       </c>
       <c r="K23" s="27" t="s">
-        <v>315</v>
+        <v>310</v>
       </c>
     </row>
     <row r="24" spans="1:25" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A24" s="24" t="s">
-        <v>303</v>
+        <v>298</v>
       </c>
       <c r="B24" s="12" t="s">
-        <v>76</v>
+        <v>74</v>
       </c>
       <c r="C24" s="25" t="s">
-        <v>316</v>
+        <v>311</v>
       </c>
       <c r="D24" s="12" t="s">
-        <v>164</v>
+        <v>159</v>
       </c>
       <c r="E24" s="12" t="s">
-        <v>317</v>
+        <v>312</v>
       </c>
       <c r="F24" s="12" t="s">
         <v>18</v>
       </c>
       <c r="G24" s="12" t="s">
-        <v>318</v>
+        <v>313</v>
       </c>
       <c r="H24" s="26" t="s">
-        <v>319</v>
+        <v>314</v>
       </c>
       <c r="I24" s="24" t="s">
-        <v>320</v>
+        <v>315</v>
       </c>
       <c r="J24" s="12" t="s">
-        <v>321</v>
+        <v>316</v>
       </c>
       <c r="K24" s="27" t="s">
-        <v>322</v>
+        <v>317</v>
       </c>
     </row>
     <row r="25" spans="1:25" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A25" s="30" t="s">
-        <v>323</v>
+        <v>318</v>
       </c>
       <c r="B25" s="31" t="s">
-        <v>79</v>
+        <v>76</v>
       </c>
       <c r="C25" s="32" t="s">
-        <v>324</v>
+        <v>319</v>
       </c>
       <c r="D25" s="31" t="s">
-        <v>185</v>
+        <v>180</v>
       </c>
       <c r="E25" s="33" t="s">
-        <v>325</v>
+        <v>320</v>
       </c>
       <c r="F25" s="31" t="s">
         <v>18</v>
       </c>
       <c r="G25" s="31" t="s">
-        <v>326</v>
+        <v>321</v>
       </c>
       <c r="H25" s="36" t="s">
-        <v>327</v>
+        <v>322</v>
       </c>
       <c r="I25" s="30" t="s">
-        <v>328</v>
+        <v>323</v>
       </c>
       <c r="J25" s="31" t="s">
-        <v>329</v>
+        <v>324</v>
       </c>
       <c r="K25" s="34" t="s">
-        <v>330</v>
+        <v>325</v>
       </c>
       <c r="L25" s="35"/>
       <c r="M25" s="35"/>
@@ -9380,37 +9380,37 @@
     </row>
     <row r="26" spans="1:25" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A26" s="30" t="s">
-        <v>323</v>
+        <v>318</v>
       </c>
       <c r="B26" s="31" t="s">
-        <v>79</v>
+        <v>76</v>
       </c>
       <c r="C26" s="32" t="s">
+        <v>326</v>
+      </c>
+      <c r="D26" s="31" t="s">
+        <v>159</v>
+      </c>
+      <c r="E26" s="31" t="s">
+        <v>327</v>
+      </c>
+      <c r="F26" s="31" t="s">
+        <v>107</v>
+      </c>
+      <c r="G26" s="31" t="s">
+        <v>328</v>
+      </c>
+      <c r="H26" s="36" t="s">
+        <v>329</v>
+      </c>
+      <c r="I26" s="30" t="s">
+        <v>330</v>
+      </c>
+      <c r="J26" s="31" t="s">
         <v>331</v>
       </c>
-      <c r="D26" s="31" t="s">
-        <v>164</v>
-      </c>
-      <c r="E26" s="31" t="s">
+      <c r="K26" s="34" t="s">
         <v>332</v>
-      </c>
-      <c r="F26" s="31" t="s">
-        <v>112</v>
-      </c>
-      <c r="G26" s="31" t="s">
-        <v>333</v>
-      </c>
-      <c r="H26" s="36" t="s">
-        <v>334</v>
-      </c>
-      <c r="I26" s="30" t="s">
-        <v>335</v>
-      </c>
-      <c r="J26" s="31" t="s">
-        <v>336</v>
-      </c>
-      <c r="K26" s="34" t="s">
-        <v>337</v>
       </c>
       <c r="L26" s="35"/>
       <c r="M26" s="35"/>
@@ -9429,107 +9429,107 @@
     </row>
     <row r="27" spans="1:25" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A27" s="24" t="s">
+        <v>333</v>
+      </c>
+      <c r="B27" s="12" t="s">
+        <v>78</v>
+      </c>
+      <c r="C27" s="25" t="s">
+        <v>334</v>
+      </c>
+      <c r="D27" s="12" t="s">
+        <v>180</v>
+      </c>
+      <c r="E27" s="3" t="s">
+        <v>335</v>
+      </c>
+      <c r="F27" s="12" t="s">
+        <v>107</v>
+      </c>
+      <c r="G27" s="12" t="s">
+        <v>336</v>
+      </c>
+      <c r="H27" s="26" t="s">
+        <v>337</v>
+      </c>
+      <c r="I27" s="24" t="s">
         <v>338</v>
       </c>
-      <c r="B27" s="12" t="s">
-        <v>81</v>
-      </c>
-      <c r="C27" s="25" t="s">
+      <c r="J27" s="12" t="s">
         <v>339</v>
       </c>
-      <c r="D27" s="12" t="s">
-        <v>185</v>
-      </c>
-      <c r="E27" s="3" t="s">
+      <c r="K27" s="27" t="s">
         <v>340</v>
-      </c>
-      <c r="F27" s="12" t="s">
-        <v>112</v>
-      </c>
-      <c r="G27" s="12" t="s">
-        <v>341</v>
-      </c>
-      <c r="H27" s="26" t="s">
-        <v>342</v>
-      </c>
-      <c r="I27" s="24" t="s">
-        <v>343</v>
-      </c>
-      <c r="J27" s="12" t="s">
-        <v>344</v>
-      </c>
-      <c r="K27" s="27" t="s">
-        <v>345</v>
       </c>
     </row>
     <row r="28" spans="1:25" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A28" s="24" t="s">
-        <v>338</v>
+        <v>333</v>
       </c>
       <c r="B28" s="12" t="s">
-        <v>81</v>
+        <v>78</v>
       </c>
       <c r="C28" s="25" t="s">
-        <v>346</v>
+        <v>341</v>
       </c>
       <c r="D28" s="12" t="s">
-        <v>164</v>
+        <v>159</v>
       </c>
       <c r="E28" s="12" t="s">
-        <v>347</v>
+        <v>342</v>
       </c>
       <c r="F28" s="12" t="s">
-        <v>177</v>
+        <v>172</v>
       </c>
       <c r="G28" s="12" t="s">
-        <v>341</v>
+        <v>336</v>
       </c>
       <c r="H28" s="26" t="s">
-        <v>342</v>
+        <v>337</v>
       </c>
       <c r="I28" s="24" t="s">
-        <v>348</v>
+        <v>343</v>
       </c>
       <c r="J28" s="12" t="s">
-        <v>349</v>
+        <v>344</v>
       </c>
       <c r="K28" s="27" t="s">
-        <v>350</v>
+        <v>345</v>
       </c>
     </row>
     <row r="29" spans="1:25" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A29" s="30" t="s">
-        <v>351</v>
+        <v>346</v>
       </c>
       <c r="B29" s="31" t="s">
-        <v>84</v>
+        <v>81</v>
       </c>
       <c r="C29" s="32" t="s">
-        <v>352</v>
+        <v>347</v>
       </c>
       <c r="D29" s="31" t="s">
-        <v>185</v>
+        <v>180</v>
       </c>
       <c r="E29" s="33" t="s">
-        <v>353</v>
+        <v>348</v>
       </c>
       <c r="F29" s="31" t="s">
         <v>18</v>
       </c>
       <c r="G29" s="31" t="s">
-        <v>354</v>
+        <v>349</v>
       </c>
       <c r="H29" s="36" t="s">
-        <v>355</v>
+        <v>350</v>
       </c>
       <c r="I29" s="30" t="s">
-        <v>356</v>
+        <v>351</v>
       </c>
       <c r="J29" s="31" t="s">
-        <v>357</v>
+        <v>352</v>
       </c>
       <c r="K29" s="34" t="s">
-        <v>358</v>
+        <v>353</v>
       </c>
       <c r="L29" s="35"/>
       <c r="M29" s="35"/>
@@ -9548,37 +9548,37 @@
     </row>
     <row r="30" spans="1:25" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A30" s="30" t="s">
-        <v>351</v>
+        <v>346</v>
       </c>
       <c r="B30" s="31" t="s">
-        <v>84</v>
+        <v>81</v>
       </c>
       <c r="C30" s="32" t="s">
-        <v>359</v>
+        <v>354</v>
       </c>
       <c r="D30" s="31" t="s">
-        <v>164</v>
+        <v>159</v>
       </c>
       <c r="E30" s="31" t="s">
-        <v>360</v>
+        <v>355</v>
       </c>
       <c r="F30" s="31" t="s">
         <v>18</v>
       </c>
       <c r="G30" s="31" t="s">
-        <v>361</v>
+        <v>356</v>
       </c>
       <c r="H30" s="36" t="s">
-        <v>362</v>
+        <v>357</v>
       </c>
       <c r="I30" s="30" t="s">
-        <v>363</v>
+        <v>358</v>
       </c>
       <c r="J30" s="31" t="s">
-        <v>364</v>
+        <v>359</v>
       </c>
       <c r="K30" s="34" t="s">
-        <v>365</v>
+        <v>360</v>
       </c>
       <c r="L30" s="35"/>
       <c r="M30" s="35"/>
@@ -9597,34 +9597,34 @@
     </row>
     <row r="31" spans="1:25" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A31" s="30" t="s">
-        <v>351</v>
+        <v>346</v>
       </c>
       <c r="B31" s="31" t="s">
-        <v>84</v>
+        <v>81</v>
       </c>
       <c r="C31" s="32" t="s">
+        <v>361</v>
+      </c>
+      <c r="D31" s="31" t="s">
+        <v>159</v>
+      </c>
+      <c r="E31" s="31" t="s">
+        <v>362</v>
+      </c>
+      <c r="F31" s="31" t="s">
+        <v>107</v>
+      </c>
+      <c r="G31" s="31" t="s">
+        <v>363</v>
+      </c>
+      <c r="H31" s="36" t="s">
+        <v>364</v>
+      </c>
+      <c r="I31" s="30" t="s">
+        <v>365</v>
+      </c>
+      <c r="J31" s="31" t="s">
         <v>366</v>
-      </c>
-      <c r="D31" s="31" t="s">
-        <v>164</v>
-      </c>
-      <c r="E31" s="31" t="s">
-        <v>367</v>
-      </c>
-      <c r="F31" s="31" t="s">
-        <v>112</v>
-      </c>
-      <c r="G31" s="31" t="s">
-        <v>368</v>
-      </c>
-      <c r="H31" s="36" t="s">
-        <v>369</v>
-      </c>
-      <c r="I31" s="30" t="s">
-        <v>370</v>
-      </c>
-      <c r="J31" s="31" t="s">
-        <v>371</v>
       </c>
       <c r="K31" s="35"/>
       <c r="L31" s="35"/>
@@ -9644,107 +9644,107 @@
     </row>
     <row r="32" spans="1:25" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A32" s="24" t="s">
-        <v>372</v>
+        <v>367</v>
       </c>
       <c r="B32" s="12" t="s">
-        <v>86</v>
+        <v>83</v>
       </c>
       <c r="C32" s="25" t="s">
-        <v>373</v>
+        <v>368</v>
       </c>
       <c r="D32" s="12" t="s">
-        <v>185</v>
+        <v>180</v>
       </c>
       <c r="E32" s="3" t="s">
-        <v>374</v>
+        <v>369</v>
       </c>
       <c r="F32" s="12" t="s">
         <v>18</v>
       </c>
       <c r="G32" s="12" t="s">
-        <v>375</v>
+        <v>370</v>
       </c>
       <c r="H32" s="26" t="s">
-        <v>376</v>
+        <v>371</v>
       </c>
       <c r="I32" s="24" t="s">
-        <v>377</v>
+        <v>372</v>
       </c>
       <c r="J32" s="12" t="s">
-        <v>281</v>
+        <v>276</v>
       </c>
       <c r="K32" s="37" t="s">
-        <v>378</v>
+        <v>373</v>
       </c>
     </row>
     <row r="33" spans="1:25" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A33" s="24" t="s">
-        <v>372</v>
+        <v>367</v>
       </c>
       <c r="B33" s="12" t="s">
-        <v>86</v>
+        <v>83</v>
       </c>
       <c r="C33" s="25" t="s">
+        <v>374</v>
+      </c>
+      <c r="D33" s="12" t="s">
+        <v>159</v>
+      </c>
+      <c r="E33" s="12" t="s">
+        <v>375</v>
+      </c>
+      <c r="F33" s="12" t="s">
+        <v>107</v>
+      </c>
+      <c r="G33" s="12" t="s">
+        <v>376</v>
+      </c>
+      <c r="H33" s="26" t="s">
+        <v>377</v>
+      </c>
+      <c r="I33" s="24" t="s">
+        <v>378</v>
+      </c>
+      <c r="J33" s="12" t="s">
         <v>379</v>
       </c>
-      <c r="D33" s="12" t="s">
-        <v>164</v>
-      </c>
-      <c r="E33" s="12" t="s">
+      <c r="K33" s="37" t="s">
         <v>380</v>
-      </c>
-      <c r="F33" s="12" t="s">
-        <v>112</v>
-      </c>
-      <c r="G33" s="12" t="s">
-        <v>381</v>
-      </c>
-      <c r="H33" s="26" t="s">
-        <v>382</v>
-      </c>
-      <c r="I33" s="24" t="s">
-        <v>383</v>
-      </c>
-      <c r="J33" s="12" t="s">
-        <v>384</v>
-      </c>
-      <c r="K33" s="37" t="s">
-        <v>385</v>
       </c>
     </row>
     <row r="34" spans="1:25" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A34" s="30" t="s">
-        <v>386</v>
+        <v>381</v>
       </c>
       <c r="B34" s="31" t="s">
-        <v>88</v>
+        <v>85</v>
       </c>
       <c r="C34" s="32" t="s">
-        <v>387</v>
+        <v>382</v>
       </c>
       <c r="D34" s="31" t="s">
-        <v>185</v>
+        <v>180</v>
       </c>
       <c r="E34" s="33" t="s">
-        <v>388</v>
+        <v>383</v>
       </c>
       <c r="F34" s="31" t="s">
         <v>18</v>
       </c>
       <c r="G34" s="31" t="s">
-        <v>389</v>
+        <v>384</v>
       </c>
       <c r="H34" s="36" t="s">
-        <v>390</v>
+        <v>385</v>
       </c>
       <c r="I34" s="30" t="s">
-        <v>391</v>
+        <v>386</v>
       </c>
       <c r="J34" s="31" t="s">
-        <v>392</v>
+        <v>387</v>
       </c>
       <c r="K34" s="38" t="s">
-        <v>393</v>
+        <v>388</v>
       </c>
       <c r="L34" s="35"/>
       <c r="M34" s="35"/>
@@ -9763,34 +9763,34 @@
     </row>
     <row r="35" spans="1:25" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A35" s="30" t="s">
-        <v>386</v>
+        <v>381</v>
       </c>
       <c r="B35" s="31" t="s">
-        <v>88</v>
+        <v>85</v>
       </c>
       <c r="C35" s="32" t="s">
+        <v>389</v>
+      </c>
+      <c r="D35" s="31" t="s">
+        <v>159</v>
+      </c>
+      <c r="E35" s="31" t="s">
+        <v>390</v>
+      </c>
+      <c r="F35" s="31" t="s">
+        <v>172</v>
+      </c>
+      <c r="G35" s="31" t="s">
+        <v>391</v>
+      </c>
+      <c r="H35" s="36" t="s">
+        <v>392</v>
+      </c>
+      <c r="I35" s="30" t="s">
+        <v>393</v>
+      </c>
+      <c r="J35" s="31" t="s">
         <v>394</v>
-      </c>
-      <c r="D35" s="31" t="s">
-        <v>164</v>
-      </c>
-      <c r="E35" s="31" t="s">
-        <v>395</v>
-      </c>
-      <c r="F35" s="31" t="s">
-        <v>177</v>
-      </c>
-      <c r="G35" s="31" t="s">
-        <v>396</v>
-      </c>
-      <c r="H35" s="36" t="s">
-        <v>397</v>
-      </c>
-      <c r="I35" s="30" t="s">
-        <v>398</v>
-      </c>
-      <c r="J35" s="31" t="s">
-        <v>399</v>
       </c>
       <c r="K35" s="35"/>
       <c r="L35" s="35"/>
@@ -9810,197 +9810,197 @@
     </row>
     <row r="36" spans="1:25" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A36" s="24" t="s">
-        <v>400</v>
+        <v>395</v>
       </c>
       <c r="B36" s="12" t="s">
-        <v>102</v>
+        <v>99</v>
       </c>
       <c r="C36" s="25" t="s">
-        <v>401</v>
+        <v>396</v>
       </c>
       <c r="D36" s="12" t="s">
-        <v>164</v>
+        <v>159</v>
       </c>
       <c r="E36" s="12" t="s">
-        <v>402</v>
+        <v>397</v>
       </c>
       <c r="F36" s="12" t="s">
         <v>18</v>
       </c>
       <c r="G36" s="12" t="s">
-        <v>403</v>
+        <v>398</v>
       </c>
       <c r="H36" s="26" t="s">
-        <v>404</v>
+        <v>399</v>
       </c>
       <c r="I36" s="24" t="s">
-        <v>405</v>
+        <v>400</v>
       </c>
       <c r="J36" s="12" t="s">
-        <v>406</v>
+        <v>401</v>
       </c>
       <c r="K36" s="37" t="s">
-        <v>407</v>
+        <v>402</v>
       </c>
     </row>
     <row r="37" spans="1:25" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A37" s="24" t="s">
-        <v>400</v>
+        <v>395</v>
       </c>
       <c r="B37" s="12" t="s">
-        <v>102</v>
+        <v>99</v>
       </c>
       <c r="C37" s="25" t="s">
-        <v>408</v>
+        <v>403</v>
       </c>
       <c r="D37" s="12" t="s">
-        <v>164</v>
+        <v>159</v>
       </c>
       <c r="E37" s="12" t="s">
-        <v>409</v>
+        <v>404</v>
       </c>
       <c r="F37" s="12" t="s">
         <v>18</v>
       </c>
       <c r="G37" s="12" t="s">
-        <v>410</v>
+        <v>405</v>
       </c>
       <c r="H37" s="26" t="s">
-        <v>411</v>
+        <v>406</v>
       </c>
       <c r="I37" s="24" t="s">
-        <v>412</v>
+        <v>407</v>
       </c>
       <c r="J37" s="12" t="s">
-        <v>413</v>
+        <v>408</v>
       </c>
       <c r="K37" s="37" t="s">
-        <v>414</v>
+        <v>409</v>
       </c>
     </row>
     <row r="38" spans="1:25" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A38" s="24" t="s">
-        <v>400</v>
+        <v>395</v>
       </c>
       <c r="B38" s="12" t="s">
-        <v>102</v>
+        <v>99</v>
       </c>
       <c r="C38" s="25" t="s">
-        <v>415</v>
+        <v>410</v>
       </c>
       <c r="D38" s="12" t="s">
-        <v>164</v>
+        <v>159</v>
       </c>
       <c r="E38" s="12" t="s">
-        <v>416</v>
+        <v>411</v>
       </c>
       <c r="F38" s="12" t="s">
         <v>18</v>
       </c>
       <c r="G38" s="12" t="s">
-        <v>417</v>
+        <v>412</v>
       </c>
       <c r="H38" s="26" t="s">
-        <v>418</v>
+        <v>413</v>
       </c>
       <c r="I38" s="24" t="s">
-        <v>419</v>
+        <v>414</v>
       </c>
     </row>
     <row r="39" spans="1:25" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A39" s="24" t="s">
-        <v>400</v>
+        <v>395</v>
       </c>
       <c r="B39" s="12" t="s">
-        <v>102</v>
+        <v>99</v>
       </c>
       <c r="C39" s="25" t="s">
-        <v>420</v>
+        <v>415</v>
       </c>
       <c r="D39" s="12" t="s">
-        <v>164</v>
+        <v>159</v>
       </c>
       <c r="E39" s="12" t="s">
-        <v>421</v>
+        <v>416</v>
       </c>
       <c r="F39" s="12" t="s">
         <v>18</v>
       </c>
       <c r="G39" s="12" t="s">
+        <v>412</v>
+      </c>
+      <c r="H39" s="26" t="s">
+        <v>413</v>
+      </c>
+      <c r="I39" s="24" t="s">
         <v>417</v>
       </c>
-      <c r="H39" s="26" t="s">
+      <c r="J39" s="12" t="s">
         <v>418</v>
       </c>
-      <c r="I39" s="24" t="s">
-        <v>422</v>
-      </c>
-      <c r="J39" s="12" t="s">
-        <v>423</v>
-      </c>
       <c r="K39" s="27" t="s">
-        <v>424</v>
+        <v>419</v>
       </c>
     </row>
     <row r="40" spans="1:25" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A40" s="24" t="s">
-        <v>400</v>
+        <v>395</v>
       </c>
       <c r="B40" s="12" t="s">
-        <v>102</v>
+        <v>99</v>
       </c>
       <c r="C40" s="25" t="s">
-        <v>425</v>
+        <v>420</v>
       </c>
       <c r="D40" s="12" t="s">
-        <v>164</v>
+        <v>159</v>
       </c>
       <c r="E40" s="12" t="s">
-        <v>426</v>
+        <v>421</v>
       </c>
       <c r="F40" s="12" t="s">
         <v>18</v>
       </c>
       <c r="G40" s="12" t="s">
-        <v>427</v>
+        <v>422</v>
       </c>
       <c r="H40" s="26" t="s">
-        <v>418</v>
+        <v>413</v>
       </c>
       <c r="I40" s="24" t="s">
-        <v>428</v>
+        <v>423</v>
       </c>
       <c r="J40" s="12" t="s">
-        <v>429</v>
+        <v>424</v>
       </c>
     </row>
     <row r="41" spans="1:25" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A41" s="30" t="s">
-        <v>430</v>
+        <v>425</v>
       </c>
       <c r="B41" s="31" t="s">
-        <v>108</v>
+        <v>104</v>
       </c>
       <c r="C41" s="32" t="s">
-        <v>431</v>
+        <v>426</v>
       </c>
       <c r="D41" s="31" t="s">
-        <v>164</v>
+        <v>159</v>
       </c>
       <c r="E41" s="31" t="s">
-        <v>432</v>
+        <v>427</v>
       </c>
       <c r="F41" s="31" t="s">
         <v>18</v>
       </c>
       <c r="G41" s="31" t="s">
-        <v>433</v>
+        <v>428</v>
       </c>
       <c r="H41" s="36" t="s">
-        <v>434</v>
+        <v>429</v>
       </c>
       <c r="I41" s="30" t="s">
-        <v>435</v>
+        <v>430</v>
       </c>
       <c r="J41" s="35"/>
       <c r="K41" s="35"/>
@@ -10021,37 +10021,37 @@
     </row>
     <row r="42" spans="1:25" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A42" s="30" t="s">
-        <v>430</v>
+        <v>425</v>
       </c>
       <c r="B42" s="31" t="s">
-        <v>108</v>
+        <v>104</v>
       </c>
       <c r="C42" s="32" t="s">
+        <v>431</v>
+      </c>
+      <c r="D42" s="31" t="s">
+        <v>180</v>
+      </c>
+      <c r="E42" s="33" t="s">
+        <v>432</v>
+      </c>
+      <c r="F42" s="31" t="s">
+        <v>107</v>
+      </c>
+      <c r="G42" s="31" t="s">
+        <v>433</v>
+      </c>
+      <c r="H42" s="36" t="s">
+        <v>434</v>
+      </c>
+      <c r="I42" s="30" t="s">
+        <v>435</v>
+      </c>
+      <c r="J42" s="31" t="s">
         <v>436</v>
       </c>
-      <c r="D42" s="31" t="s">
-        <v>185</v>
-      </c>
-      <c r="E42" s="33" t="s">
+      <c r="K42" s="34" t="s">
         <v>437</v>
-      </c>
-      <c r="F42" s="31" t="s">
-        <v>112</v>
-      </c>
-      <c r="G42" s="31" t="s">
-        <v>438</v>
-      </c>
-      <c r="H42" s="36" t="s">
-        <v>439</v>
-      </c>
-      <c r="I42" s="30" t="s">
-        <v>440</v>
-      </c>
-      <c r="J42" s="31" t="s">
-        <v>441</v>
-      </c>
-      <c r="K42" s="34" t="s">
-        <v>442</v>
       </c>
       <c r="L42" s="35"/>
       <c r="M42" s="35"/>
@@ -10070,34 +10070,34 @@
     </row>
     <row r="43" spans="1:25" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A43" s="30" t="s">
-        <v>430</v>
+        <v>425</v>
       </c>
       <c r="B43" s="31" t="s">
-        <v>108</v>
+        <v>104</v>
       </c>
       <c r="C43" s="32" t="s">
+        <v>438</v>
+      </c>
+      <c r="D43" s="31" t="s">
+        <v>159</v>
+      </c>
+      <c r="E43" s="31" t="s">
+        <v>439</v>
+      </c>
+      <c r="F43" s="31" t="s">
+        <v>107</v>
+      </c>
+      <c r="G43" s="31" t="s">
+        <v>440</v>
+      </c>
+      <c r="H43" s="36" t="s">
+        <v>441</v>
+      </c>
+      <c r="I43" s="30" t="s">
+        <v>442</v>
+      </c>
+      <c r="J43" s="31" t="s">
         <v>443</v>
-      </c>
-      <c r="D43" s="31" t="s">
-        <v>164</v>
-      </c>
-      <c r="E43" s="31" t="s">
-        <v>444</v>
-      </c>
-      <c r="F43" s="31" t="s">
-        <v>112</v>
-      </c>
-      <c r="G43" s="31" t="s">
-        <v>445</v>
-      </c>
-      <c r="H43" s="36" t="s">
-        <v>446</v>
-      </c>
-      <c r="I43" s="30" t="s">
-        <v>447</v>
-      </c>
-      <c r="J43" s="31" t="s">
-        <v>448</v>
       </c>
       <c r="K43" s="35"/>
       <c r="L43" s="35"/>
@@ -10117,89 +10117,89 @@
     </row>
     <row r="44" spans="1:25" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A44" s="24" t="s">
-        <v>449</v>
+        <v>444</v>
       </c>
       <c r="B44" s="12" t="s">
-        <v>114</v>
+        <v>109</v>
       </c>
       <c r="C44" s="25" t="s">
-        <v>450</v>
+        <v>445</v>
       </c>
       <c r="D44" s="12" t="s">
-        <v>185</v>
+        <v>180</v>
       </c>
       <c r="E44" s="3" t="s">
-        <v>451</v>
+        <v>446</v>
       </c>
       <c r="F44" s="12" t="s">
         <v>18</v>
       </c>
       <c r="G44" s="12" t="s">
-        <v>452</v>
+        <v>447</v>
       </c>
       <c r="H44" s="26" t="s">
-        <v>453</v>
+        <v>448</v>
       </c>
       <c r="I44" s="24" t="s">
-        <v>454</v>
+        <v>449</v>
       </c>
     </row>
     <row r="45" spans="1:25" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A45" s="24" t="s">
-        <v>449</v>
+        <v>444</v>
       </c>
       <c r="B45" s="12" t="s">
-        <v>114</v>
+        <v>109</v>
       </c>
       <c r="C45" s="25" t="s">
-        <v>455</v>
+        <v>450</v>
       </c>
       <c r="D45" s="12" t="s">
-        <v>164</v>
+        <v>159</v>
       </c>
       <c r="E45" s="12" t="s">
-        <v>456</v>
+        <v>451</v>
       </c>
       <c r="F45" s="12" t="s">
-        <v>112</v>
+        <v>107</v>
       </c>
       <c r="G45" s="12" t="s">
-        <v>457</v>
+        <v>452</v>
       </c>
       <c r="H45" s="26" t="s">
-        <v>458</v>
+        <v>453</v>
       </c>
       <c r="I45" s="24" t="s">
-        <v>459</v>
+        <v>454</v>
       </c>
     </row>
     <row r="46" spans="1:25" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A46" s="30" t="s">
-        <v>460</v>
+        <v>455</v>
       </c>
       <c r="B46" s="31" t="s">
-        <v>116</v>
+        <v>111</v>
       </c>
       <c r="C46" s="32" t="s">
-        <v>461</v>
+        <v>456</v>
       </c>
       <c r="D46" s="31" t="s">
-        <v>185</v>
+        <v>180</v>
       </c>
       <c r="E46" s="33" t="s">
-        <v>462</v>
+        <v>457</v>
       </c>
       <c r="F46" s="31" t="s">
         <v>18</v>
       </c>
       <c r="G46" s="31" t="s">
-        <v>463</v>
+        <v>458</v>
       </c>
       <c r="H46" s="36" t="s">
-        <v>464</v>
+        <v>459</v>
       </c>
       <c r="I46" s="30" t="s">
-        <v>465</v>
+        <v>460</v>
       </c>
       <c r="J46" s="35"/>
       <c r="K46" s="35"/>
@@ -10220,31 +10220,31 @@
     </row>
     <row r="47" spans="1:25" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A47" s="30" t="s">
-        <v>460</v>
+        <v>455</v>
       </c>
       <c r="B47" s="31" t="s">
-        <v>116</v>
+        <v>111</v>
       </c>
       <c r="C47" s="32" t="s">
-        <v>466</v>
+        <v>461</v>
       </c>
       <c r="D47" s="31" t="s">
-        <v>164</v>
+        <v>159</v>
       </c>
       <c r="E47" s="31" t="s">
-        <v>467</v>
+        <v>462</v>
       </c>
       <c r="F47" s="31" t="s">
         <v>18</v>
       </c>
       <c r="G47" s="31" t="s">
-        <v>468</v>
+        <v>463</v>
       </c>
       <c r="H47" s="36" t="s">
-        <v>469</v>
+        <v>464</v>
       </c>
       <c r="I47" s="30" t="s">
-        <v>470</v>
+        <v>465</v>
       </c>
       <c r="J47" s="35"/>
       <c r="K47" s="35"/>
@@ -10265,31 +10265,31 @@
     </row>
     <row r="48" spans="1:25" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A48" s="30" t="s">
-        <v>460</v>
+        <v>455</v>
       </c>
       <c r="B48" s="31" t="s">
-        <v>116</v>
+        <v>111</v>
       </c>
       <c r="C48" s="32" t="s">
-        <v>471</v>
+        <v>466</v>
       </c>
       <c r="D48" s="31" t="s">
-        <v>164</v>
+        <v>159</v>
       </c>
       <c r="E48" s="31" t="s">
-        <v>472</v>
+        <v>467</v>
       </c>
       <c r="F48" s="31" t="s">
-        <v>112</v>
+        <v>107</v>
       </c>
       <c r="G48" s="31" t="s">
-        <v>473</v>
+        <v>468</v>
       </c>
       <c r="H48" s="36" t="s">
-        <v>474</v>
+        <v>469</v>
       </c>
       <c r="I48" s="30" t="s">
-        <v>447</v>
+        <v>442</v>
       </c>
       <c r="J48" s="35"/>
       <c r="K48" s="35"/>
@@ -10310,118 +10310,118 @@
     </row>
     <row r="49" spans="1:25" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A49" s="24" t="s">
-        <v>475</v>
+        <v>470</v>
       </c>
       <c r="B49" s="12" t="s">
-        <v>120</v>
+        <v>115</v>
       </c>
       <c r="C49" s="25" t="s">
-        <v>476</v>
+        <v>471</v>
       </c>
       <c r="D49" s="12" t="s">
-        <v>185</v>
+        <v>180</v>
       </c>
       <c r="E49" s="3" t="s">
-        <v>477</v>
+        <v>472</v>
       </c>
       <c r="F49" s="12" t="s">
         <v>18</v>
       </c>
       <c r="G49" s="12" t="s">
-        <v>478</v>
+        <v>473</v>
       </c>
       <c r="H49" s="26" t="s">
-        <v>479</v>
+        <v>474</v>
       </c>
       <c r="I49" s="24" t="s">
-        <v>480</v>
+        <v>475</v>
       </c>
     </row>
     <row r="50" spans="1:25" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A50" s="24" t="s">
-        <v>475</v>
+        <v>470</v>
       </c>
       <c r="B50" s="12" t="s">
-        <v>120</v>
+        <v>115</v>
       </c>
       <c r="C50" s="25" t="s">
-        <v>481</v>
+        <v>476</v>
       </c>
       <c r="D50" s="12" t="s">
-        <v>164</v>
+        <v>159</v>
       </c>
       <c r="E50" s="12" t="s">
-        <v>482</v>
+        <v>477</v>
       </c>
       <c r="F50" s="12" t="s">
         <v>18</v>
       </c>
       <c r="G50" s="12" t="s">
-        <v>468</v>
+        <v>463</v>
       </c>
       <c r="H50" s="26" t="s">
-        <v>469</v>
+        <v>464</v>
       </c>
       <c r="I50" s="24" t="s">
-        <v>483</v>
+        <v>478</v>
       </c>
     </row>
     <row r="51" spans="1:25" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A51" s="24" t="s">
-        <v>475</v>
+        <v>470</v>
       </c>
       <c r="B51" s="12" t="s">
-        <v>120</v>
+        <v>115</v>
       </c>
       <c r="C51" s="25" t="s">
-        <v>484</v>
+        <v>479</v>
       </c>
       <c r="D51" s="12" t="s">
-        <v>164</v>
+        <v>159</v>
       </c>
       <c r="E51" s="12" t="s">
-        <v>485</v>
+        <v>480</v>
       </c>
       <c r="F51" s="12" t="s">
-        <v>112</v>
+        <v>107</v>
       </c>
       <c r="G51" s="12" t="s">
-        <v>433</v>
+        <v>428</v>
       </c>
       <c r="H51" s="26" t="s">
-        <v>434</v>
+        <v>429</v>
       </c>
       <c r="I51" s="24" t="s">
-        <v>486</v>
+        <v>481</v>
       </c>
     </row>
     <row r="52" spans="1:25" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A52" s="30" t="s">
-        <v>487</v>
+        <v>482</v>
       </c>
       <c r="B52" s="31" t="s">
-        <v>125</v>
+        <v>120</v>
       </c>
       <c r="C52" s="32" t="s">
-        <v>488</v>
+        <v>483</v>
       </c>
       <c r="D52" s="31" t="s">
-        <v>185</v>
+        <v>180</v>
       </c>
       <c r="E52" s="33" t="s">
-        <v>489</v>
+        <v>484</v>
       </c>
       <c r="F52" s="31" t="s">
         <v>18</v>
       </c>
       <c r="G52" s="31" t="s">
-        <v>490</v>
+        <v>485</v>
       </c>
       <c r="H52" s="36" t="s">
-        <v>491</v>
+        <v>486</v>
       </c>
       <c r="I52" s="30" t="s">
-        <v>492</v>
+        <v>487</v>
       </c>
       <c r="J52" s="35"/>
       <c r="K52" s="35"/>
@@ -10442,31 +10442,31 @@
     </row>
     <row r="53" spans="1:25" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A53" s="30" t="s">
-        <v>487</v>
+        <v>482</v>
       </c>
       <c r="B53" s="31" t="s">
-        <v>125</v>
+        <v>120</v>
       </c>
       <c r="C53" s="32" t="s">
-        <v>493</v>
+        <v>488</v>
       </c>
       <c r="D53" s="31" t="s">
-        <v>164</v>
+        <v>159</v>
       </c>
       <c r="E53" s="31" t="s">
-        <v>494</v>
+        <v>489</v>
       </c>
       <c r="F53" s="31" t="s">
-        <v>177</v>
+        <v>172</v>
       </c>
       <c r="G53" s="31" t="s">
-        <v>495</v>
+        <v>490</v>
       </c>
       <c r="H53" s="36" t="s">
-        <v>496</v>
+        <v>491</v>
       </c>
       <c r="I53" s="30" t="s">
-        <v>483</v>
+        <v>478</v>
       </c>
       <c r="J53" s="35"/>
       <c r="K53" s="35"/>
@@ -10487,89 +10487,89 @@
     </row>
     <row r="54" spans="1:25" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A54" s="24" t="s">
-        <v>497</v>
+        <v>492</v>
       </c>
       <c r="B54" s="12" t="s">
-        <v>127</v>
+        <v>122</v>
       </c>
       <c r="C54" s="25" t="s">
-        <v>498</v>
+        <v>493</v>
       </c>
       <c r="D54" s="12" t="s">
-        <v>185</v>
+        <v>180</v>
       </c>
       <c r="E54" s="3" t="s">
-        <v>499</v>
+        <v>494</v>
       </c>
       <c r="F54" s="12" t="s">
         <v>18</v>
       </c>
       <c r="G54" s="12" t="s">
-        <v>500</v>
+        <v>495</v>
       </c>
       <c r="H54" s="26" t="s">
-        <v>501</v>
+        <v>496</v>
       </c>
       <c r="I54" s="24" t="s">
-        <v>502</v>
+        <v>497</v>
       </c>
     </row>
     <row r="55" spans="1:25" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A55" s="24" t="s">
-        <v>497</v>
+        <v>492</v>
       </c>
       <c r="B55" s="12" t="s">
-        <v>127</v>
+        <v>122</v>
       </c>
       <c r="C55" s="25" t="s">
-        <v>503</v>
+        <v>498</v>
       </c>
       <c r="D55" s="12" t="s">
-        <v>164</v>
+        <v>159</v>
       </c>
       <c r="E55" s="12" t="s">
-        <v>504</v>
+        <v>499</v>
       </c>
       <c r="F55" s="12" t="s">
-        <v>112</v>
+        <v>107</v>
       </c>
       <c r="G55" s="12" t="s">
+        <v>495</v>
+      </c>
+      <c r="H55" s="26" t="s">
+        <v>496</v>
+      </c>
+      <c r="I55" s="24" t="s">
         <v>500</v>
-      </c>
-      <c r="H55" s="26" t="s">
-        <v>501</v>
-      </c>
-      <c r="I55" s="24" t="s">
-        <v>505</v>
       </c>
     </row>
     <row r="56" spans="1:25" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A56" s="30" t="s">
-        <v>506</v>
+        <v>501</v>
       </c>
       <c r="B56" s="31" t="s">
-        <v>131</v>
+        <v>126</v>
       </c>
       <c r="C56" s="32" t="s">
-        <v>507</v>
+        <v>502</v>
       </c>
       <c r="D56" s="31" t="s">
-        <v>185</v>
+        <v>180</v>
       </c>
       <c r="E56" s="33" t="s">
-        <v>508</v>
+        <v>503</v>
       </c>
       <c r="F56" s="31" t="s">
         <v>18</v>
       </c>
       <c r="G56" s="31" t="s">
-        <v>509</v>
+        <v>504</v>
       </c>
       <c r="H56" s="36" t="s">
-        <v>510</v>
+        <v>505</v>
       </c>
       <c r="I56" s="30" t="s">
-        <v>511</v>
+        <v>506</v>
       </c>
       <c r="J56" s="35"/>
       <c r="K56" s="35"/>
@@ -10590,31 +10590,31 @@
     </row>
     <row r="57" spans="1:25" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A57" s="30" t="s">
-        <v>506</v>
+        <v>501</v>
       </c>
       <c r="B57" s="31" t="s">
-        <v>131</v>
+        <v>126</v>
       </c>
       <c r="C57" s="32" t="s">
-        <v>512</v>
+        <v>507</v>
       </c>
       <c r="D57" s="31" t="s">
-        <v>164</v>
+        <v>159</v>
       </c>
       <c r="E57" s="31" t="s">
-        <v>513</v>
+        <v>508</v>
       </c>
       <c r="F57" s="31" t="s">
-        <v>112</v>
+        <v>107</v>
       </c>
       <c r="G57" s="31" t="s">
-        <v>514</v>
+        <v>509</v>
       </c>
       <c r="H57" s="36" t="s">
-        <v>515</v>
+        <v>510</v>
       </c>
       <c r="I57" s="30" t="s">
-        <v>287</v>
+        <v>282</v>
       </c>
       <c r="J57" s="35"/>
       <c r="K57" s="35"/>
@@ -10635,89 +10635,89 @@
     </row>
     <row r="58" spans="1:25" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A58" s="24" t="s">
-        <v>516</v>
+        <v>511</v>
       </c>
       <c r="B58" s="12" t="s">
-        <v>137</v>
+        <v>132</v>
       </c>
       <c r="C58" s="25" t="s">
-        <v>517</v>
+        <v>512</v>
       </c>
       <c r="D58" s="12" t="s">
-        <v>185</v>
+        <v>180</v>
       </c>
       <c r="E58" s="3" t="s">
-        <v>518</v>
+        <v>513</v>
       </c>
       <c r="F58" s="12" t="s">
         <v>18</v>
       </c>
       <c r="G58" s="12" t="s">
-        <v>519</v>
+        <v>514</v>
       </c>
       <c r="H58" s="26" t="s">
-        <v>520</v>
+        <v>515</v>
       </c>
       <c r="I58" s="24" t="s">
-        <v>521</v>
+        <v>516</v>
       </c>
     </row>
     <row r="59" spans="1:25" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A59" s="24" t="s">
-        <v>516</v>
+        <v>511</v>
       </c>
       <c r="B59" s="12" t="s">
-        <v>137</v>
+        <v>132</v>
       </c>
       <c r="C59" s="25" t="s">
-        <v>522</v>
+        <v>517</v>
       </c>
       <c r="D59" s="12" t="s">
-        <v>164</v>
+        <v>159</v>
       </c>
       <c r="E59" s="12" t="s">
-        <v>523</v>
+        <v>518</v>
       </c>
       <c r="F59" s="12" t="s">
-        <v>112</v>
+        <v>107</v>
       </c>
       <c r="G59" s="12" t="s">
-        <v>524</v>
+        <v>519</v>
       </c>
       <c r="H59" s="26" t="s">
-        <v>525</v>
+        <v>520</v>
       </c>
       <c r="I59" s="24" t="s">
-        <v>526</v>
+        <v>521</v>
       </c>
     </row>
     <row r="60" spans="1:25" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A60" s="30" t="s">
-        <v>527</v>
+        <v>522</v>
       </c>
       <c r="B60" s="31" t="s">
-        <v>139</v>
+        <v>134</v>
       </c>
       <c r="C60" s="32" t="s">
-        <v>528</v>
+        <v>523</v>
       </c>
       <c r="D60" s="31" t="s">
-        <v>185</v>
+        <v>180</v>
       </c>
       <c r="E60" s="33" t="s">
-        <v>529</v>
+        <v>524</v>
       </c>
       <c r="F60" s="31" t="s">
         <v>18</v>
       </c>
       <c r="G60" s="31" t="s">
-        <v>530</v>
+        <v>525</v>
       </c>
       <c r="H60" s="36" t="s">
-        <v>531</v>
+        <v>526</v>
       </c>
       <c r="I60" s="30" t="s">
-        <v>532</v>
+        <v>527</v>
       </c>
       <c r="J60" s="35"/>
       <c r="K60" s="35"/>
@@ -10738,31 +10738,31 @@
     </row>
     <row r="61" spans="1:25" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A61" s="30" t="s">
-        <v>527</v>
+        <v>522</v>
       </c>
       <c r="B61" s="31" t="s">
-        <v>139</v>
+        <v>134</v>
       </c>
       <c r="C61" s="32" t="s">
-        <v>533</v>
+        <v>528</v>
       </c>
       <c r="D61" s="31" t="s">
-        <v>164</v>
+        <v>159</v>
       </c>
       <c r="E61" s="31" t="s">
-        <v>534</v>
+        <v>529</v>
       </c>
       <c r="F61" s="31" t="s">
-        <v>112</v>
+        <v>107</v>
       </c>
       <c r="G61" s="31" t="s">
-        <v>535</v>
+        <v>530</v>
       </c>
       <c r="H61" s="36" t="s">
-        <v>536</v>
+        <v>531</v>
       </c>
       <c r="I61" s="30" t="s">
-        <v>398</v>
+        <v>393</v>
       </c>
       <c r="J61" s="35"/>
       <c r="K61" s="35"/>
@@ -10783,31 +10783,31 @@
     </row>
     <row r="62" spans="1:25" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A62" s="30" t="s">
-        <v>527</v>
+        <v>522</v>
       </c>
       <c r="B62" s="31" t="s">
-        <v>139</v>
+        <v>134</v>
       </c>
       <c r="C62" s="32" t="s">
-        <v>537</v>
+        <v>532</v>
       </c>
       <c r="D62" s="31" t="s">
-        <v>164</v>
+        <v>159</v>
       </c>
       <c r="E62" s="31" t="s">
-        <v>538</v>
+        <v>533</v>
       </c>
       <c r="F62" s="31" t="s">
-        <v>112</v>
+        <v>107</v>
       </c>
       <c r="G62" s="31" t="s">
-        <v>539</v>
+        <v>534</v>
       </c>
       <c r="H62" s="36" t="s">
-        <v>540</v>
+        <v>535</v>
       </c>
       <c r="I62" s="30" t="s">
-        <v>541</v>
+        <v>536</v>
       </c>
       <c r="J62" s="35"/>
       <c r="K62" s="35"/>
@@ -15595,25 +15595,25 @@
         <v>1</v>
       </c>
       <c r="C1" s="3" t="s">
-        <v>154</v>
+        <v>149</v>
       </c>
       <c r="D1" s="3" t="s">
         <v>7</v>
       </c>
       <c r="E1" s="3" t="s">
-        <v>155</v>
+        <v>150</v>
       </c>
       <c r="F1" s="3" t="s">
-        <v>156</v>
+        <v>151</v>
       </c>
       <c r="G1" s="3" t="s">
-        <v>157</v>
+        <v>152</v>
       </c>
       <c r="H1" s="3" t="s">
-        <v>158</v>
+        <v>153</v>
       </c>
       <c r="I1" s="3" t="s">
-        <v>159</v>
+        <v>154</v>
       </c>
       <c r="J1" s="9"/>
       <c r="K1" s="9"/>
@@ -15634,466 +15634,466 @@
     </row>
     <row r="2" spans="1:25" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A2" s="26" t="s">
-        <v>542</v>
+        <v>537</v>
       </c>
       <c r="B2" s="12" t="s">
         <v>24</v>
       </c>
       <c r="C2" s="26" t="s">
-        <v>543</v>
+        <v>538</v>
       </c>
       <c r="D2" s="12" t="s">
-        <v>185</v>
+        <v>180</v>
       </c>
       <c r="E2" s="12" t="s">
-        <v>544</v>
+        <v>539</v>
       </c>
       <c r="F2" s="12" t="s">
         <v>18</v>
       </c>
       <c r="G2" s="12" t="s">
-        <v>545</v>
+        <v>540</v>
       </c>
       <c r="H2" s="26" t="s">
-        <v>546</v>
+        <v>541</v>
       </c>
       <c r="I2" s="26" t="s">
-        <v>547</v>
+        <v>542</v>
       </c>
     </row>
     <row r="3" spans="1:25" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A3" s="26" t="s">
-        <v>548</v>
+        <v>543</v>
       </c>
       <c r="B3" s="12" t="s">
-        <v>32</v>
+        <v>31</v>
       </c>
       <c r="C3" s="26" t="s">
-        <v>549</v>
+        <v>544</v>
       </c>
       <c r="D3" s="12" t="s">
-        <v>185</v>
+        <v>180</v>
       </c>
       <c r="E3" s="12" t="s">
-        <v>550</v>
+        <v>545</v>
       </c>
       <c r="F3" s="12" t="s">
         <v>18</v>
       </c>
       <c r="G3" s="12" t="s">
-        <v>551</v>
+        <v>546</v>
       </c>
       <c r="H3" s="26" t="s">
-        <v>552</v>
+        <v>547</v>
       </c>
       <c r="I3" s="26" t="s">
-        <v>553</v>
+        <v>548</v>
       </c>
     </row>
     <row r="4" spans="1:25" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A4" s="26" t="s">
+        <v>549</v>
+      </c>
+      <c r="B4" s="12" t="s">
+        <v>38</v>
+      </c>
+      <c r="C4" s="26" t="s">
+        <v>550</v>
+      </c>
+      <c r="D4" s="12" t="s">
+        <v>180</v>
+      </c>
+      <c r="E4" s="12" t="s">
+        <v>551</v>
+      </c>
+      <c r="F4" s="12" t="s">
+        <v>107</v>
+      </c>
+      <c r="G4" s="12" t="s">
+        <v>552</v>
+      </c>
+      <c r="H4" s="26" t="s">
+        <v>553</v>
+      </c>
+      <c r="I4" s="26" t="s">
         <v>554</v>
-      </c>
-      <c r="B4" s="12" t="s">
-        <v>39</v>
-      </c>
-      <c r="C4" s="26" t="s">
-        <v>555</v>
-      </c>
-      <c r="D4" s="12" t="s">
-        <v>185</v>
-      </c>
-      <c r="E4" s="12" t="s">
-        <v>556</v>
-      </c>
-      <c r="F4" s="12" t="s">
-        <v>112</v>
-      </c>
-      <c r="G4" s="12" t="s">
-        <v>557</v>
-      </c>
-      <c r="H4" s="26" t="s">
-        <v>558</v>
-      </c>
-      <c r="I4" s="26" t="s">
-        <v>559</v>
       </c>
     </row>
     <row r="5" spans="1:25" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A5" s="26" t="s">
-        <v>560</v>
+        <v>555</v>
       </c>
       <c r="B5" s="12" t="s">
-        <v>44</v>
+        <v>43</v>
       </c>
       <c r="C5" s="26" t="s">
-        <v>561</v>
+        <v>556</v>
       </c>
       <c r="D5" s="12" t="s">
-        <v>185</v>
+        <v>180</v>
       </c>
       <c r="E5" s="12" t="s">
-        <v>562</v>
+        <v>557</v>
       </c>
       <c r="F5" s="12" t="s">
         <v>18</v>
       </c>
       <c r="G5" s="12" t="s">
-        <v>563</v>
+        <v>558</v>
       </c>
       <c r="H5" s="26" t="s">
-        <v>564</v>
+        <v>559</v>
       </c>
       <c r="I5" s="26" t="s">
-        <v>565</v>
+        <v>560</v>
       </c>
     </row>
     <row r="6" spans="1:25" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A6" s="26" t="s">
-        <v>566</v>
+        <v>561</v>
       </c>
       <c r="B6" s="12" t="s">
-        <v>53</v>
+        <v>51</v>
       </c>
       <c r="C6" s="26" t="s">
-        <v>567</v>
+        <v>562</v>
       </c>
       <c r="D6" s="12" t="s">
-        <v>185</v>
+        <v>180</v>
       </c>
       <c r="E6" s="12" t="s">
-        <v>568</v>
+        <v>563</v>
       </c>
       <c r="F6" s="12" t="s">
         <v>18</v>
       </c>
       <c r="G6" s="12" t="s">
-        <v>569</v>
+        <v>564</v>
       </c>
       <c r="H6" s="26" t="s">
-        <v>570</v>
+        <v>565</v>
       </c>
       <c r="I6" s="26" t="s">
-        <v>571</v>
+        <v>566</v>
       </c>
     </row>
     <row r="7" spans="1:25" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A7" s="26" t="s">
-        <v>572</v>
+        <v>567</v>
       </c>
       <c r="B7" s="12" t="s">
-        <v>58</v>
+        <v>56</v>
       </c>
       <c r="C7" s="26" t="s">
-        <v>573</v>
+        <v>568</v>
       </c>
       <c r="D7" s="12" t="s">
-        <v>185</v>
+        <v>180</v>
       </c>
       <c r="E7" s="12" t="s">
-        <v>574</v>
+        <v>569</v>
       </c>
       <c r="F7" s="12" t="s">
         <v>18</v>
       </c>
       <c r="G7" s="12" t="s">
-        <v>575</v>
+        <v>570</v>
       </c>
       <c r="H7" s="26" t="s">
-        <v>576</v>
+        <v>571</v>
       </c>
       <c r="I7" s="26" t="s">
-        <v>577</v>
+        <v>572</v>
       </c>
     </row>
     <row r="8" spans="1:25" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A8" s="26" t="s">
-        <v>578</v>
+        <v>573</v>
       </c>
       <c r="B8" s="12" t="s">
-        <v>65</v>
+        <v>63</v>
       </c>
       <c r="C8" s="26" t="s">
-        <v>579</v>
+        <v>574</v>
       </c>
       <c r="D8" s="12" t="s">
-        <v>185</v>
+        <v>180</v>
       </c>
       <c r="E8" s="12" t="s">
-        <v>580</v>
+        <v>575</v>
       </c>
       <c r="F8" s="12" t="s">
         <v>18</v>
       </c>
       <c r="G8" s="12" t="s">
-        <v>581</v>
+        <v>576</v>
       </c>
       <c r="H8" s="26" t="s">
-        <v>582</v>
+        <v>577</v>
       </c>
       <c r="I8" s="26" t="s">
-        <v>583</v>
+        <v>578</v>
       </c>
     </row>
     <row r="9" spans="1:25" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A9" s="26" t="s">
-        <v>584</v>
+        <v>579</v>
       </c>
       <c r="B9" s="12" t="s">
-        <v>67</v>
+        <v>65</v>
       </c>
       <c r="C9" s="26" t="s">
-        <v>585</v>
+        <v>580</v>
       </c>
       <c r="D9" s="12" t="s">
-        <v>185</v>
+        <v>180</v>
       </c>
       <c r="E9" s="12" t="s">
-        <v>586</v>
+        <v>581</v>
       </c>
       <c r="F9" s="12" t="s">
         <v>18</v>
       </c>
       <c r="G9" s="12" t="s">
-        <v>587</v>
+        <v>582</v>
       </c>
       <c r="H9" s="26" t="s">
-        <v>588</v>
+        <v>583</v>
       </c>
       <c r="I9" s="26" t="s">
-        <v>589</v>
+        <v>584</v>
       </c>
     </row>
     <row r="10" spans="1:25" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A10" s="26" t="s">
-        <v>590</v>
+        <v>585</v>
       </c>
       <c r="B10" s="12" t="s">
-        <v>70</v>
+        <v>68</v>
       </c>
       <c r="C10" s="26" t="s">
-        <v>591</v>
+        <v>586</v>
       </c>
       <c r="D10" s="12" t="s">
-        <v>185</v>
+        <v>180</v>
       </c>
       <c r="E10" s="12" t="s">
-        <v>592</v>
+        <v>587</v>
       </c>
       <c r="F10" s="12" t="s">
         <v>18</v>
       </c>
       <c r="G10" s="12" t="s">
-        <v>593</v>
+        <v>588</v>
       </c>
       <c r="H10" s="26" t="s">
-        <v>594</v>
+        <v>589</v>
       </c>
       <c r="I10" s="26" t="s">
-        <v>595</v>
+        <v>590</v>
       </c>
     </row>
     <row r="11" spans="1:25" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A11" s="26" t="s">
-        <v>596</v>
+        <v>591</v>
       </c>
       <c r="B11" s="12" t="s">
-        <v>74</v>
+        <v>72</v>
       </c>
       <c r="C11" s="26" t="s">
-        <v>597</v>
+        <v>592</v>
       </c>
       <c r="D11" s="12" t="s">
-        <v>185</v>
+        <v>180</v>
       </c>
       <c r="E11" s="12" t="s">
-        <v>598</v>
+        <v>593</v>
       </c>
       <c r="F11" s="12" t="s">
         <v>18</v>
       </c>
       <c r="G11" s="12" t="s">
-        <v>599</v>
+        <v>594</v>
       </c>
       <c r="H11" s="12" t="s">
-        <v>600</v>
+        <v>595</v>
       </c>
       <c r="I11" s="26" t="s">
-        <v>601</v>
+        <v>596</v>
       </c>
     </row>
     <row r="12" spans="1:25" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A12" s="26" t="s">
-        <v>602</v>
+        <v>597</v>
       </c>
       <c r="B12" s="12" t="s">
-        <v>91</v>
+        <v>88</v>
       </c>
       <c r="C12" s="26" t="s">
-        <v>603</v>
+        <v>598</v>
       </c>
       <c r="D12" s="12" t="s">
-        <v>185</v>
+        <v>180</v>
       </c>
       <c r="E12" s="12" t="s">
-        <v>604</v>
+        <v>599</v>
       </c>
       <c r="F12" s="12" t="s">
         <v>18</v>
       </c>
       <c r="G12" s="12" t="s">
-        <v>417</v>
+        <v>412</v>
       </c>
       <c r="H12" s="26" t="s">
-        <v>605</v>
+        <v>600</v>
       </c>
       <c r="I12" s="26" t="s">
-        <v>606</v>
+        <v>601</v>
       </c>
     </row>
     <row r="13" spans="1:25" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A13" s="26" t="s">
-        <v>607</v>
+        <v>602</v>
       </c>
       <c r="B13" s="12" t="s">
-        <v>95</v>
+        <v>92</v>
       </c>
       <c r="C13" s="26" t="s">
-        <v>608</v>
+        <v>603</v>
       </c>
       <c r="D13" s="12" t="s">
-        <v>185</v>
+        <v>180</v>
       </c>
       <c r="E13" s="12" t="s">
-        <v>609</v>
+        <v>604</v>
       </c>
       <c r="F13" s="12" t="s">
         <v>18</v>
       </c>
       <c r="G13" s="12" t="s">
-        <v>610</v>
+        <v>605</v>
       </c>
       <c r="H13" s="26" t="s">
-        <v>611</v>
+        <v>606</v>
       </c>
       <c r="I13" s="26" t="s">
-        <v>612</v>
+        <v>607</v>
       </c>
     </row>
     <row r="14" spans="1:25" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A14" s="26" t="s">
-        <v>613</v>
+        <v>608</v>
       </c>
       <c r="B14" s="12" t="s">
-        <v>97</v>
+        <v>94</v>
       </c>
       <c r="C14" s="26" t="s">
-        <v>614</v>
+        <v>609</v>
       </c>
       <c r="D14" s="12" t="s">
-        <v>185</v>
+        <v>180</v>
       </c>
       <c r="E14" s="12" t="s">
-        <v>615</v>
+        <v>610</v>
       </c>
       <c r="F14" s="12" t="s">
         <v>18</v>
       </c>
       <c r="G14" s="12" t="s">
-        <v>616</v>
+        <v>611</v>
       </c>
       <c r="H14" s="26" t="s">
-        <v>617</v>
+        <v>612</v>
       </c>
       <c r="I14" s="26" t="s">
-        <v>618</v>
+        <v>613</v>
       </c>
     </row>
     <row r="15" spans="1:25" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A15" s="26" t="s">
-        <v>619</v>
+        <v>614</v>
       </c>
       <c r="B15" s="12" t="s">
-        <v>99</v>
+        <v>96</v>
       </c>
       <c r="C15" s="26" t="s">
-        <v>620</v>
+        <v>615</v>
       </c>
       <c r="D15" s="12" t="s">
-        <v>185</v>
+        <v>180</v>
       </c>
       <c r="E15" s="12" t="s">
-        <v>621</v>
+        <v>616</v>
       </c>
       <c r="F15" s="12" t="s">
         <v>18</v>
       </c>
       <c r="G15" s="12" t="s">
-        <v>622</v>
+        <v>617</v>
       </c>
       <c r="H15" s="26" t="s">
-        <v>623</v>
+        <v>618</v>
       </c>
       <c r="I15" s="26" t="s">
-        <v>624</v>
+        <v>619</v>
       </c>
     </row>
     <row r="16" spans="1:25" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A16" s="26" t="s">
-        <v>625</v>
+        <v>620</v>
       </c>
       <c r="B16" s="12" t="s">
-        <v>105</v>
+        <v>101</v>
       </c>
       <c r="C16" s="26" t="s">
-        <v>626</v>
+        <v>621</v>
       </c>
       <c r="D16" s="12" t="s">
-        <v>185</v>
+        <v>180</v>
       </c>
       <c r="E16" s="12" t="s">
-        <v>627</v>
+        <v>622</v>
       </c>
       <c r="F16" s="12" t="s">
         <v>18</v>
       </c>
       <c r="G16" s="12" t="s">
-        <v>628</v>
+        <v>623</v>
       </c>
       <c r="H16" s="26" t="s">
-        <v>629</v>
+        <v>624</v>
       </c>
       <c r="I16" s="26" t="s">
-        <v>630</v>
+        <v>625</v>
       </c>
     </row>
     <row r="17" spans="1:9" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A17" s="26" t="s">
-        <v>631</v>
+        <v>626</v>
       </c>
       <c r="B17" s="12" t="s">
-        <v>134</v>
+        <v>129</v>
       </c>
       <c r="C17" s="26" t="s">
-        <v>632</v>
+        <v>627</v>
       </c>
       <c r="D17" s="12" t="s">
-        <v>185</v>
+        <v>180</v>
       </c>
       <c r="E17" s="12" t="s">
-        <v>633</v>
+        <v>628</v>
       </c>
       <c r="F17" s="12" t="s">
         <v>18</v>
       </c>
       <c r="G17" s="12" t="s">
-        <v>634</v>
+        <v>629</v>
       </c>
       <c r="H17" s="26" t="s">
-        <v>635</v>
+        <v>630</v>
       </c>
       <c r="I17" s="26" t="s">
-        <v>636</v>
+        <v>631</v>
       </c>
     </row>
   </sheetData>

</xml_diff>